<commit_message>
Excel is now without errors.
</commit_message>
<xml_diff>
--- a/TraysFastUpdate/wwwroot/Trays.xlsx
+++ b/TraysFastUpdate/wwwroot/Trays.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trays" sheetId="1" r:id="R2807d9a52f12492d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trays" sheetId="1" r:id="R00e26a0dcbfe4fbe"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -68,7 +68,7 @@
       <x:c r="F2" t="n">
         <x:v>7838.070</x:v>
       </x:c>
-      <x:c r="G2" t="n">
+      <x:c r="G2" t="str">
         <x:v>75.67</x:v>
       </x:c>
     </x:row>
@@ -91,7 +91,7 @@
       <x:c r="F3" t="n">
         <x:v>23600.619</x:v>
       </x:c>
-      <x:c r="G3" t="n">
+      <x:c r="G3" t="str">
         <x:v>63.60</x:v>
       </x:c>
     </x:row>
@@ -114,7 +114,7 @@
       <x:c r="F4" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G4" t="n">
+      <x:c r="G4" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -137,7 +137,7 @@
       <x:c r="F5" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G5" t="n">
+      <x:c r="G5" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -160,7 +160,7 @@
       <x:c r="F6" t="n">
         <x:v>1700.619</x:v>
       </x:c>
-      <x:c r="G6" t="n">
+      <x:c r="G6" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -183,7 +183,7 @@
       <x:c r="F7" t="n">
         <x:v>1700.619</x:v>
       </x:c>
-      <x:c r="G7" t="n">
+      <x:c r="G7" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -206,7 +206,7 @@
       <x:c r="F8" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G8" t="n">
+      <x:c r="G8" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -229,7 +229,7 @@
       <x:c r="F9" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G9" t="n">
+      <x:c r="G9" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -252,7 +252,7 @@
       <x:c r="F10" t="n">
         <x:v>6325.284</x:v>
       </x:c>
-      <x:c r="G10" t="n">
+      <x:c r="G10" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -275,7 +275,7 @@
       <x:c r="F11" t="n">
         <x:v>6325.284</x:v>
       </x:c>
-      <x:c r="G11" t="n">
+      <x:c r="G11" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -298,7 +298,7 @@
       <x:c r="F12" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G12" t="n">
+      <x:c r="G12" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -321,7 +321,7 @@
       <x:c r="F13" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G13" t="n">
+      <x:c r="G13" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -344,7 +344,7 @@
       <x:c r="F14" t="n">
         <x:v>5764.057</x:v>
       </x:c>
-      <x:c r="G14" t="n">
+      <x:c r="G14" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -367,7 +367,7 @@
       <x:c r="F15" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G15" t="n">
+      <x:c r="G15" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -390,7 +390,7 @@
       <x:c r="F16" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G16" t="n">
+      <x:c r="G16" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -413,7 +413,7 @@
       <x:c r="F17" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G17" t="n">
+      <x:c r="G17" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -436,7 +436,7 @@
       <x:c r="F18" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G18" t="n">
+      <x:c r="G18" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -459,7 +459,7 @@
       <x:c r="F19" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G19" t="n">
+      <x:c r="G19" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -482,7 +482,7 @@
       <x:c r="F20" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G20" t="n">
+      <x:c r="G20" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -505,7 +505,7 @@
       <x:c r="F21" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G21" t="n">
+      <x:c r="G21" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -528,7 +528,7 @@
       <x:c r="F22" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G22" t="n">
+      <x:c r="G22" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -551,7 +551,7 @@
       <x:c r="F23" t="n">
         <x:v>11439.220</x:v>
       </x:c>
-      <x:c r="G23" t="n">
+      <x:c r="G23" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -574,7 +574,7 @@
       <x:c r="F24" t="n">
         <x:v>11439.220</x:v>
       </x:c>
-      <x:c r="G24" t="n">
+      <x:c r="G24" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -597,7 +597,7 @@
       <x:c r="F25" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G25" t="n">
+      <x:c r="G25" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -620,7 +620,7 @@
       <x:c r="F26" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G26" t="n">
+      <x:c r="G26" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -643,7 +643,7 @@
       <x:c r="F27" t="n">
         <x:v>5642.599</x:v>
       </x:c>
-      <x:c r="G27" t="n">
+      <x:c r="G27" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -666,7 +666,7 @@
       <x:c r="F28" t="n">
         <x:v>5643.821</x:v>
       </x:c>
-      <x:c r="G28" t="n">
+      <x:c r="G28" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -689,7 +689,7 @@
       <x:c r="F29" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G29" t="n">
+      <x:c r="G29" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -712,7 +712,7 @@
       <x:c r="F30" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G30" t="n">
+      <x:c r="G30" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -735,7 +735,7 @@
       <x:c r="F31" t="n">
         <x:v>1800.000</x:v>
       </x:c>
-      <x:c r="G31" t="n">
+      <x:c r="G31" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -758,7 +758,7 @@
       <x:c r="F32" t="n">
         <x:v>1800.000</x:v>
       </x:c>
-      <x:c r="G32" t="n">
+      <x:c r="G32" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -781,7 +781,7 @@
       <x:c r="F33" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G33" t="n">
+      <x:c r="G33" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -804,7 +804,7 @@
       <x:c r="F34" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G34" t="n">
+      <x:c r="G34" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -827,7 +827,7 @@
       <x:c r="F35" t="n">
         <x:v>5830.812</x:v>
       </x:c>
-      <x:c r="G35" t="n">
+      <x:c r="G35" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -850,7 +850,7 @@
       <x:c r="F36" t="n">
         <x:v>5830.812</x:v>
       </x:c>
-      <x:c r="G36" t="n">
+      <x:c r="G36" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -873,7 +873,7 @@
       <x:c r="F37" t="n">
         <x:v>4970.900</x:v>
       </x:c>
-      <x:c r="G37" t="n">
+      <x:c r="G37" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -896,7 +896,7 @@
       <x:c r="F38" t="n">
         <x:v>11174.950</x:v>
       </x:c>
-      <x:c r="G38" t="n">
+      <x:c r="G38" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -919,7 +919,7 @@
       <x:c r="F39" t="n">
         <x:v>10327.774</x:v>
       </x:c>
-      <x:c r="G39" t="n">
+      <x:c r="G39" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -942,7 +942,7 @@
       <x:c r="F40" t="n">
         <x:v>25905.369</x:v>
       </x:c>
-      <x:c r="G40" t="n">
+      <x:c r="G40" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -965,7 +965,7 @@
       <x:c r="F41" t="n">
         <x:v>25105.369</x:v>
       </x:c>
-      <x:c r="G41" t="n">
+      <x:c r="G41" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -988,7 +988,7 @@
       <x:c r="F42" t="n">
         <x:v>10326.481</x:v>
       </x:c>
-      <x:c r="G42" t="n">
+      <x:c r="G42" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1011,7 +1011,7 @@
       <x:c r="F43" t="n">
         <x:v>11174.424</x:v>
       </x:c>
-      <x:c r="G43" t="n">
+      <x:c r="G43" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1034,7 +1034,7 @@
       <x:c r="F44" t="n">
         <x:v>4218.868</x:v>
       </x:c>
-      <x:c r="G44" t="n">
+      <x:c r="G44" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1057,7 +1057,7 @@
       <x:c r="F45" t="n">
         <x:v>5764.057</x:v>
       </x:c>
-      <x:c r="G45" t="n">
+      <x:c r="G45" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1080,7 +1080,7 @@
       <x:c r="F46" t="n">
         <x:v>5642.620</x:v>
       </x:c>
-      <x:c r="G46" t="n">
+      <x:c r="G46" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1103,7 +1103,7 @@
       <x:c r="F47" t="n">
         <x:v>5642.620</x:v>
       </x:c>
-      <x:c r="G47" t="n">
+      <x:c r="G47" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1126,7 +1126,7 @@
       <x:c r="F48" t="n">
         <x:v>7736.447</x:v>
       </x:c>
-      <x:c r="G48" t="n">
+      <x:c r="G48" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1149,7 +1149,7 @@
       <x:c r="F49" t="n">
         <x:v>7736.447</x:v>
       </x:c>
-      <x:c r="G49" t="n">
+      <x:c r="G49" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1172,7 +1172,7 @@
       <x:c r="F50" t="n">
         <x:v>10433.601</x:v>
       </x:c>
-      <x:c r="G50" t="n">
+      <x:c r="G50" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1195,7 +1195,7 @@
       <x:c r="F51" t="n">
         <x:v>10433.601</x:v>
       </x:c>
-      <x:c r="G51" t="n">
+      <x:c r="G51" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1218,7 +1218,7 @@
       <x:c r="F52" t="n">
         <x:v>6912.929</x:v>
       </x:c>
-      <x:c r="G52" t="n">
+      <x:c r="G52" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1241,7 +1241,7 @@
       <x:c r="F53" t="n">
         <x:v>7062.451</x:v>
       </x:c>
-      <x:c r="G53" t="n">
+      <x:c r="G53" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1264,7 +1264,7 @@
       <x:c r="F54" t="n">
         <x:v>6912.929</x:v>
       </x:c>
-      <x:c r="G54" t="n">
+      <x:c r="G54" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1287,7 +1287,7 @@
       <x:c r="F55" t="n">
         <x:v>6968.311</x:v>
       </x:c>
-      <x:c r="G55" t="n">
+      <x:c r="G55" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1310,7 +1310,7 @@
       <x:c r="F56" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G56" t="n">
+      <x:c r="G56" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1333,7 +1333,7 @@
       <x:c r="F57" t="n">
         <x:v>4725.000</x:v>
       </x:c>
-      <x:c r="G57" t="n">
+      <x:c r="G57" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1356,7 +1356,7 @@
       <x:c r="F58" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G58" t="n">
+      <x:c r="G58" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1379,7 +1379,7 @@
       <x:c r="F59" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G59" t="n">
+      <x:c r="G59" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1402,7 +1402,7 @@
       <x:c r="F60" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G60" t="n">
+      <x:c r="G60" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1425,7 +1425,7 @@
       <x:c r="F61" t="n">
         <x:v>5025.000</x:v>
       </x:c>
-      <x:c r="G61" t="n">
+      <x:c r="G61" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1448,7 +1448,7 @@
       <x:c r="F62" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G62" t="n">
+      <x:c r="G62" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1471,7 +1471,7 @@
       <x:c r="F63" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G63" t="n">
+      <x:c r="G63" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1494,7 +1494,7 @@
       <x:c r="F64" t="n">
         <x:v>6894.960</x:v>
       </x:c>
-      <x:c r="G64" t="n">
+      <x:c r="G64" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1517,7 +1517,7 @@
       <x:c r="F65" t="n">
         <x:v>7084.929</x:v>
       </x:c>
-      <x:c r="G65" t="n">
+      <x:c r="G65" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1540,7 +1540,7 @@
       <x:c r="F66" t="n">
         <x:v>6962.449</x:v>
       </x:c>
-      <x:c r="G66" t="n">
+      <x:c r="G66" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1563,7 +1563,7 @@
       <x:c r="F67" t="n">
         <x:v>7084.929</x:v>
       </x:c>
-      <x:c r="G67" t="n">
+      <x:c r="G67" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1586,7 +1586,7 @@
       <x:c r="F68" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G68" t="n">
+      <x:c r="G68" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1609,7 +1609,7 @@
       <x:c r="F69" t="n">
         <x:v>5025.000</x:v>
       </x:c>
-      <x:c r="G69" t="n">
+      <x:c r="G69" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1632,7 +1632,7 @@
       <x:c r="F70" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G70" t="n">
+      <x:c r="G70" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1655,7 +1655,7 @@
       <x:c r="F71" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G71" t="n">
+      <x:c r="G71" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1678,7 +1678,7 @@
       <x:c r="F72" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G72" t="n">
+      <x:c r="G72" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1701,7 +1701,7 @@
       <x:c r="F73" t="n">
         <x:v>5125.000</x:v>
       </x:c>
-      <x:c r="G73" t="n">
+      <x:c r="G73" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1724,7 +1724,7 @@
       <x:c r="F74" t="n">
         <x:v>2700.000</x:v>
       </x:c>
-      <x:c r="G74" t="n">
+      <x:c r="G74" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1747,7 +1747,7 @@
       <x:c r="F75" t="n">
         <x:v>2700.000</x:v>
       </x:c>
-      <x:c r="G75" t="n">
+      <x:c r="G75" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1770,7 +1770,7 @@
       <x:c r="F76" t="n">
         <x:v>21256.580</x:v>
       </x:c>
-      <x:c r="G76" t="n">
+      <x:c r="G76" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1793,7 +1793,7 @@
       <x:c r="F77" t="n">
         <x:v>20637.837</x:v>
       </x:c>
-      <x:c r="G77" t="n">
+      <x:c r="G77" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1816,7 +1816,7 @@
       <x:c r="F78" t="n">
         <x:v>22200.718</x:v>
       </x:c>
-      <x:c r="G78" t="n">
+      <x:c r="G78" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1839,7 +1839,7 @@
       <x:c r="F79" t="n">
         <x:v>21286.580</x:v>
       </x:c>
-      <x:c r="G79" t="n">
+      <x:c r="G79" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1862,7 +1862,7 @@
       <x:c r="F80" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G80" t="n">
+      <x:c r="G80" t="str">
         <x:v>38.65</x:v>
       </x:c>
     </x:row>
@@ -1885,7 +1885,7 @@
       <x:c r="F81" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G81" t="n">
+      <x:c r="G81" t="str">
         <x:v>63.47</x:v>
       </x:c>
     </x:row>
@@ -1908,7 +1908,7 @@
       <x:c r="F82" t="n">
         <x:v>7159.229</x:v>
       </x:c>
-      <x:c r="G82" t="n">
+      <x:c r="G82" t="str">
         <x:v>72.53</x:v>
       </x:c>
     </x:row>
@@ -1931,7 +1931,7 @@
       <x:c r="F83" t="n">
         <x:v>3250.000</x:v>
       </x:c>
-      <x:c r="G83" t="n">
+      <x:c r="G83" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
@@ -1954,7 +1954,7 @@
       <x:c r="F84" t="n">
         <x:v>1900.000</x:v>
       </x:c>
-      <x:c r="G84" t="n">
+      <x:c r="G84" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
@@ -1977,7 +1977,7 @@
       <x:c r="F85" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G85" t="n">
+      <x:c r="G85" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -2000,7 +2000,7 @@
       <x:c r="F86" t="n">
         <x:v>3606.000</x:v>
       </x:c>
-      <x:c r="G86" t="n">
+      <x:c r="G86" t="str">
         <x:v>34.87</x:v>
       </x:c>
     </x:row>
@@ -2023,7 +2023,7 @@
       <x:c r="F87" t="n">
         <x:v>8778.319</x:v>
       </x:c>
-      <x:c r="G87" t="n">
+      <x:c r="G87" t="str">
         <x:v>67.07</x:v>
       </x:c>
     </x:row>
@@ -2046,7 +2046,7 @@
       <x:c r="F88" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G88" t="n">
+      <x:c r="G88" t="str">
         <x:v>89.85</x:v>
       </x:c>
     </x:row>
@@ -2069,7 +2069,7 @@
       <x:c r="F89" t="n">
         <x:v>3032.809</x:v>
       </x:c>
-      <x:c r="G89" t="n">
+      <x:c r="G89" t="str">
         <x:v>37.40</x:v>
       </x:c>
     </x:row>
@@ -2092,7 +2092,7 @@
       <x:c r="F90" t="n">
         <x:v>6501.881</x:v>
       </x:c>
-      <x:c r="G90" t="n">
+      <x:c r="G90" t="str">
         <x:v>51.33</x:v>
       </x:c>
     </x:row>
@@ -2115,7 +2115,7 @@
       <x:c r="F91" t="n">
         <x:v>1196.290</x:v>
       </x:c>
-      <x:c r="G91" t="n">
+      <x:c r="G91" t="str">
         <x:v>43.13</x:v>
       </x:c>
     </x:row>
@@ -2138,7 +2138,7 @@
       <x:c r="F92" t="n">
         <x:v>1879.028</x:v>
       </x:c>
-      <x:c r="G92" t="n">
+      <x:c r="G92" t="str">
         <x:v>67.95</x:v>
       </x:c>
     </x:row>
@@ -2161,7 +2161,7 @@
       <x:c r="F93" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G93" t="n">
+      <x:c r="G93" t="str">
         <x:v>49.80</x:v>
       </x:c>
     </x:row>
@@ -2184,7 +2184,7 @@
       <x:c r="F94" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G94" t="n">
+      <x:c r="G94" t="str">
         <x:v>57.73</x:v>
       </x:c>
     </x:row>
@@ -2207,7 +2207,7 @@
       <x:c r="F95" t="n">
         <x:v>7909.844</x:v>
       </x:c>
-      <x:c r="G95" t="n">
+      <x:c r="G95" t="str">
         <x:v>62.22</x:v>
       </x:c>
     </x:row>
@@ -2230,7 +2230,7 @@
       <x:c r="F96" t="n">
         <x:v>1926.448</x:v>
       </x:c>
-      <x:c r="G96" t="n">
+      <x:c r="G96" t="str">
         <x:v>72.32</x:v>
       </x:c>
     </x:row>
@@ -2253,7 +2253,7 @@
       <x:c r="F97" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G97" t="n">
+      <x:c r="G97" t="str">
         <x:v>72.32</x:v>
       </x:c>
     </x:row>
@@ -2276,7 +2276,7 @@
       <x:c r="F98" t="n">
         <x:v>4872.000</x:v>
       </x:c>
-      <x:c r="G98" t="n">
+      <x:c r="G98" t="str">
         <x:v>76.80</x:v>
       </x:c>
     </x:row>
@@ -2299,7 +2299,7 @@
       <x:c r="F99" t="n">
         <x:v>9001.937</x:v>
       </x:c>
-      <x:c r="G99" t="n">
+      <x:c r="G99" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2322,7 +2322,7 @@
       <x:c r="F100" t="n">
         <x:v>8951.937</x:v>
       </x:c>
-      <x:c r="G100" t="n">
+      <x:c r="G100" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2345,7 +2345,7 @@
       <x:c r="F101" t="n">
         <x:v>7926.000</x:v>
       </x:c>
-      <x:c r="G101" t="n">
+      <x:c r="G101" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2368,7 +2368,7 @@
       <x:c r="F102" t="n">
         <x:v>12000.000</x:v>
       </x:c>
-      <x:c r="G102" t="n">
+      <x:c r="G102" t="str">
         <x:v>75.05</x:v>
       </x:c>
     </x:row>
@@ -2391,7 +2391,7 @@
       <x:c r="F103" t="n">
         <x:v>5638.090</x:v>
       </x:c>
-      <x:c r="G103" t="n">
+      <x:c r="G103" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
@@ -2414,7 +2414,7 @@
       <x:c r="F104" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G104" t="n">
+      <x:c r="G104" t="str">
         <x:v>73.42</x:v>
       </x:c>
     </x:row>
@@ -2437,7 +2437,7 @@
       <x:c r="F105" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G105" t="n">
+      <x:c r="G105" t="str">
         <x:v>76.97</x:v>
       </x:c>
     </x:row>
@@ -2460,7 +2460,7 @@
       <x:c r="F106" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G106" t="n">
+      <x:c r="G106" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2483,7 +2483,7 @@
       <x:c r="F107" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G107" t="n">
+      <x:c r="G107" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2506,7 +2506,7 @@
       <x:c r="F108" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G108" t="n">
+      <x:c r="G108" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2529,7 +2529,7 @@
       <x:c r="F109" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G109" t="n">
+      <x:c r="G109" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2552,7 +2552,7 @@
       <x:c r="F110" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G110" t="n">
+      <x:c r="G110" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2575,7 +2575,7 @@
       <x:c r="F111" t="n">
         <x:v>4251.206</x:v>
       </x:c>
-      <x:c r="G111" t="n">
+      <x:c r="G111" t="str">
         <x:v>57.27</x:v>
       </x:c>
     </x:row>
@@ -2598,7 +2598,7 @@
       <x:c r="F112" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G112" t="n">
+      <x:c r="G112" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2621,7 +2621,7 @@
       <x:c r="F113" t="n">
         <x:v>3706.090</x:v>
       </x:c>
-      <x:c r="G113" t="n">
+      <x:c r="G113" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2644,7 +2644,7 @@
       <x:c r="F114" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G114" t="n">
+      <x:c r="G114" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2667,7 +2667,7 @@
       <x:c r="F115" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G115" t="n">
+      <x:c r="G115" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2690,7 +2690,7 @@
       <x:c r="F116" t="n">
         <x:v>7909.844</x:v>
       </x:c>
-      <x:c r="G116" t="n">
+      <x:c r="G116" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2713,7 +2713,7 @@
       <x:c r="F117" t="n">
         <x:v>1926.448</x:v>
       </x:c>
-      <x:c r="G117" t="n">
+      <x:c r="G117" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2736,7 +2736,7 @@
       <x:c r="F118" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G118" t="n">
+      <x:c r="G118" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -2759,7 +2759,7 @@
       <x:c r="F119" t="n">
         <x:v>4067.961</x:v>
       </x:c>
-      <x:c r="G119" t="n">
+      <x:c r="G119" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -2782,7 +2782,7 @@
       <x:c r="F120" t="n">
         <x:v>1537.693</x:v>
       </x:c>
-      <x:c r="G120" t="n">
+      <x:c r="G120" t="str">
         <x:v>60.58</x:v>
       </x:c>
     </x:row>
@@ -2805,7 +2805,7 @@
       <x:c r="F121" t="n">
         <x:v>6678.620</x:v>
       </x:c>
-      <x:c r="G121" t="n">
+      <x:c r="G121" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2828,7 +2828,7 @@
       <x:c r="F122" t="n">
         <x:v>13117.566</x:v>
       </x:c>
-      <x:c r="G122" t="n">
+      <x:c r="G122" t="str">
         <x:v>57.13</x:v>
       </x:c>
     </x:row>
@@ -2851,7 +2851,7 @@
       <x:c r="F123" t="n">
         <x:v>14559.495</x:v>
       </x:c>
-      <x:c r="G123" t="n">
+      <x:c r="G123" t="str">
         <x:v>79.38</x:v>
       </x:c>
     </x:row>
@@ -2874,7 +2874,7 @@
       <x:c r="F124" t="n">
         <x:v>4919.273</x:v>
       </x:c>
-      <x:c r="G124" t="n">
+      <x:c r="G124" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2897,7 +2897,7 @@
       <x:c r="F125" t="n">
         <x:v>3890.930</x:v>
       </x:c>
-      <x:c r="G125" t="n">
+      <x:c r="G125" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2920,7 +2920,7 @@
       <x:c r="F126" t="n">
         <x:v>2807.996</x:v>
       </x:c>
-      <x:c r="G126" t="n">
+      <x:c r="G126" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2943,7 +2943,7 @@
       <x:c r="F127" t="n">
         <x:v>4100.000</x:v>
       </x:c>
-      <x:c r="G127" t="n">
+      <x:c r="G127" t="str">
         <x:v>61.80</x:v>
       </x:c>
     </x:row>
@@ -2966,7 +2966,7 @@
       <x:c r="F128" t="n">
         <x:v>6465.000</x:v>
       </x:c>
-      <x:c r="G128" t="n">
+      <x:c r="G128" t="str">
         <x:v>59.37</x:v>
       </x:c>
     </x:row>
@@ -2989,7 +2989,7 @@
       <x:c r="F129" t="n">
         <x:v>9500.000</x:v>
       </x:c>
-      <x:c r="G129" t="n">
+      <x:c r="G129" t="str">
         <x:v>57.40</x:v>
       </x:c>
     </x:row>
@@ -3012,7 +3012,7 @@
       <x:c r="F130" t="n">
         <x:v>4400.000</x:v>
       </x:c>
-      <x:c r="G130" t="n">
+      <x:c r="G130" t="str">
         <x:v>57.40</x:v>
       </x:c>
     </x:row>
@@ -3035,7 +3035,7 @@
       <x:c r="F131" t="n">
         <x:v>4703.319</x:v>
       </x:c>
-      <x:c r="G131" t="n">
+      <x:c r="G131" t="str">
         <x:v>87.43</x:v>
       </x:c>
     </x:row>
@@ -3058,7 +3058,7 @@
       <x:c r="F132" t="n">
         <x:v>4375.000</x:v>
       </x:c>
-      <x:c r="G132" t="n">
+      <x:c r="G132" t="str">
         <x:v>61.85</x:v>
       </x:c>
     </x:row>
@@ -3081,7 +3081,7 @@
       <x:c r="F133" t="n">
         <x:v>12016.902</x:v>
       </x:c>
-      <x:c r="G133" t="n">
+      <x:c r="G133" t="str">
         <x:v>93.30</x:v>
       </x:c>
     </x:row>
@@ -3104,7 +3104,7 @@
       <x:c r="F134" t="n">
         <x:v>6719.875</x:v>
       </x:c>
-      <x:c r="G134" t="n">
+      <x:c r="G134" t="str">
         <x:v>64.70</x:v>
       </x:c>
     </x:row>
@@ -3127,7 +3127,7 @@
       <x:c r="F135" t="n">
         <x:v>2915.000</x:v>
       </x:c>
-      <x:c r="G135" t="n">
+      <x:c r="G135" t="str">
         <x:v>64.70</x:v>
       </x:c>
     </x:row>
@@ -3150,7 +3150,7 @@
       <x:c r="F136" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G136" t="n">
+      <x:c r="G136" t="str">
         <x:v>72.40</x:v>
       </x:c>
     </x:row>
@@ -3173,7 +3173,7 @@
       <x:c r="F137" t="n">
         <x:v>4157.061</x:v>
       </x:c>
-      <x:c r="G137" t="n">
+      <x:c r="G137" t="str">
         <x:v>77.20</x:v>
       </x:c>
     </x:row>
@@ -3196,7 +3196,7 @@
       <x:c r="F138" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G138" t="n">
+      <x:c r="G138" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3219,7 +3219,7 @@
       <x:c r="F139" t="n">
         <x:v>4768.319</x:v>
       </x:c>
-      <x:c r="G139" t="n">
+      <x:c r="G139" t="str">
         <x:v>53.63</x:v>
       </x:c>
     </x:row>
@@ -3242,7 +3242,7 @@
       <x:c r="F140" t="n">
         <x:v>6897.001</x:v>
       </x:c>
-      <x:c r="G140" t="n">
+      <x:c r="G140" t="str">
         <x:v>76.17</x:v>
       </x:c>
     </x:row>
@@ -3265,7 +3265,7 @@
       <x:c r="F141" t="n">
         <x:v>6897.001</x:v>
       </x:c>
-      <x:c r="G141" t="n">
+      <x:c r="G141" t="str">
         <x:v>76.17</x:v>
       </x:c>
     </x:row>
@@ -3288,7 +3288,7 @@
       <x:c r="F142" t="n">
         <x:v>5709.616</x:v>
       </x:c>
-      <x:c r="G142" t="n">
+      <x:c r="G142" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3311,7 +3311,7 @@
       <x:c r="F143" t="n">
         <x:v>4953.004</x:v>
       </x:c>
-      <x:c r="G143" t="n">
+      <x:c r="G143" t="str">
         <x:v>70.90</x:v>
       </x:c>
     </x:row>
@@ -3334,7 +3334,7 @@
       <x:c r="F144" t="n">
         <x:v>6976.506</x:v>
       </x:c>
-      <x:c r="G144" t="n">
+      <x:c r="G144" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3357,7 +3357,7 @@
       <x:c r="F145" t="n">
         <x:v>4953.004</x:v>
       </x:c>
-      <x:c r="G145" t="n">
+      <x:c r="G145" t="str">
         <x:v>70.90</x:v>
       </x:c>
     </x:row>
@@ -3380,7 +3380,7 @@
       <x:c r="F146" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G146" t="n">
+      <x:c r="G146" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3403,7 +3403,7 @@
       <x:c r="F147" t="n">
         <x:v>11830.897</x:v>
       </x:c>
-      <x:c r="G147" t="n">
+      <x:c r="G147" t="str">
         <x:v>71.45</x:v>
       </x:c>
     </x:row>
@@ -3426,7 +3426,7 @@
       <x:c r="F148" t="n">
         <x:v>8464.870</x:v>
       </x:c>
-      <x:c r="G148" t="n">
+      <x:c r="G148" t="str">
         <x:v>81.92</x:v>
       </x:c>
     </x:row>
@@ -3449,7 +3449,7 @@
       <x:c r="F149" t="n">
         <x:v>4750.000</x:v>
       </x:c>
-      <x:c r="G149" t="n">
+      <x:c r="G149" t="str">
         <x:v>87.70</x:v>
       </x:c>
     </x:row>
@@ -3472,7 +3472,7 @@
       <x:c r="F150" t="n">
         <x:v>3307.715</x:v>
       </x:c>
-      <x:c r="G150" t="n">
+      <x:c r="G150" t="str">
         <x:v>90.87</x:v>
       </x:c>
     </x:row>
@@ -3495,7 +3495,7 @@
       <x:c r="F151" t="n">
         <x:v>5472.466</x:v>
       </x:c>
-      <x:c r="G151" t="n">
+      <x:c r="G151" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -3518,7 +3518,7 @@
       <x:c r="F152" t="n">
         <x:v>7241.491</x:v>
       </x:c>
-      <x:c r="G152" t="n">
+      <x:c r="G152" t="str">
         <x:v>81.33</x:v>
       </x:c>
     </x:row>
@@ -3541,7 +3541,7 @@
       <x:c r="F153" t="n">
         <x:v>3007.715</x:v>
       </x:c>
-      <x:c r="G153" t="n">
+      <x:c r="G153" t="str">
         <x:v>90.87</x:v>
       </x:c>
     </x:row>
@@ -3564,7 +3564,7 @@
       <x:c r="F154" t="n">
         <x:v>5120.505</x:v>
       </x:c>
-      <x:c r="G154" t="n">
+      <x:c r="G154" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -3587,7 +3587,7 @@
       <x:c r="F155" t="n">
         <x:v>7884.910</x:v>
       </x:c>
-      <x:c r="G155" t="n">
+      <x:c r="G155" t="str">
         <x:v>81.33</x:v>
       </x:c>
     </x:row>
@@ -3610,7 +3610,7 @@
       <x:c r="F156" t="n">
         <x:v>18778.629</x:v>
       </x:c>
-      <x:c r="G156" t="n">
+      <x:c r="G156" t="str">
         <x:v>77.72</x:v>
       </x:c>
     </x:row>
@@ -3633,7 +3633,7 @@
       <x:c r="F157" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G157" t="n">
+      <x:c r="G157" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -3656,7 +3656,7 @@
       <x:c r="F158" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G158" t="n">
+      <x:c r="G158" t="str">
         <x:v>72.65</x:v>
       </x:c>
     </x:row>
@@ -3679,7 +3679,7 @@
       <x:c r="F159" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G159" t="n">
+      <x:c r="G159" t="str">
         <x:v>77.97</x:v>
       </x:c>
     </x:row>
@@ -3702,7 +3702,7 @@
       <x:c r="F160" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G160" t="n">
+      <x:c r="G160" t="str">
         <x:v>82.52</x:v>
       </x:c>
     </x:row>
@@ -3725,7 +3725,7 @@
       <x:c r="F161" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G161" t="n">
+      <x:c r="G161" t="str">
         <x:v>79.08</x:v>
       </x:c>
     </x:row>
@@ -3748,7 +3748,7 @@
       <x:c r="F162" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G162" t="n">
+      <x:c r="G162" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -3771,7 +3771,7 @@
       <x:c r="F163" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G163" t="n">
+      <x:c r="G163" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -3794,7 +3794,7 @@
       <x:c r="F164" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G164" t="n">
+      <x:c r="G164" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -3817,7 +3817,7 @@
       <x:c r="F165" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G165" t="n">
+      <x:c r="G165" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -3840,7 +3840,7 @@
       <x:c r="F166" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G166" t="n">
+      <x:c r="G166" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -3863,7 +3863,7 @@
       <x:c r="F167" t="n">
         <x:v>8465.297</x:v>
       </x:c>
-      <x:c r="G167" t="n">
+      <x:c r="G167" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -3886,7 +3886,7 @@
       <x:c r="F168" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G168" t="n">
+      <x:c r="G168" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -3909,7 +3909,7 @@
       <x:c r="F169" t="n">
         <x:v>6974.644</x:v>
       </x:c>
-      <x:c r="G169" t="n">
+      <x:c r="G169" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -3932,7 +3932,7 @@
       <x:c r="F170" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G170" t="n">
+      <x:c r="G170" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -3955,7 +3955,7 @@
       <x:c r="F171" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G171" t="n">
+      <x:c r="G171" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -3978,7 +3978,7 @@
       <x:c r="F172" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G172" t="n">
+      <x:c r="G172" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4001,7 +4001,7 @@
       <x:c r="F173" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G173" t="n">
+      <x:c r="G173" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -4024,7 +4024,7 @@
       <x:c r="F174" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G174" t="n">
+      <x:c r="G174" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -4047,7 +4047,7 @@
       <x:c r="F175" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G175" t="n">
+      <x:c r="G175" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -4070,7 +4070,7 @@
       <x:c r="F176" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G176" t="n">
+      <x:c r="G176" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -4093,7 +4093,7 @@
       <x:c r="F177" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G177" t="n">
+      <x:c r="G177" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -4116,7 +4116,7 @@
       <x:c r="F178" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G178" t="n">
+      <x:c r="G178" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -4139,7 +4139,7 @@
       <x:c r="F179" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G179" t="n">
+      <x:c r="G179" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -4162,7 +4162,7 @@
       <x:c r="F180" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G180" t="n">
+      <x:c r="G180" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4185,7 +4185,7 @@
       <x:c r="F181" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G181" t="n">
+      <x:c r="G181" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -4208,7 +4208,7 @@
       <x:c r="F182" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G182" t="n">
+      <x:c r="G182" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -4231,7 +4231,7 @@
       <x:c r="F183" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G183" t="n">
+      <x:c r="G183" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -4254,7 +4254,7 @@
       <x:c r="F184" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G184" t="n">
+      <x:c r="G184" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -4277,7 +4277,7 @@
       <x:c r="F185" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G185" t="n">
+      <x:c r="G185" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -4300,7 +4300,7 @@
       <x:c r="F186" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G186" t="n">
+      <x:c r="G186" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -4323,7 +4323,7 @@
       <x:c r="F187" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G187" t="n">
+      <x:c r="G187" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -4346,7 +4346,7 @@
       <x:c r="F188" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G188" t="n">
+      <x:c r="G188" t="str">
         <x:v>50.62</x:v>
       </x:c>
     </x:row>
@@ -4369,7 +4369,7 @@
       <x:c r="F189" t="n">
         <x:v>4800.000</x:v>
       </x:c>
-      <x:c r="G189" t="n">
+      <x:c r="G189" t="str">
         <x:v>61.70</x:v>
       </x:c>
     </x:row>
@@ -4392,7 +4392,7 @@
       <x:c r="F190" t="n">
         <x:v>5853.750</x:v>
       </x:c>
-      <x:c r="G190" t="n">
+      <x:c r="G190" t="str">
         <x:v>71.77</x:v>
       </x:c>
     </x:row>
@@ -4415,7 +4415,7 @@
       <x:c r="F191" t="n">
         <x:v>4956.000</x:v>
       </x:c>
-      <x:c r="G191" t="n">
+      <x:c r="G191" t="str">
         <x:v>76.70</x:v>
       </x:c>
     </x:row>
@@ -4438,7 +4438,7 @@
       <x:c r="F192" t="n">
         <x:v>5424.940</x:v>
       </x:c>
-      <x:c r="G192" t="n">
+      <x:c r="G192" t="str">
         <x:v>47.08</x:v>
       </x:c>
     </x:row>
@@ -4461,7 +4461,7 @@
       <x:c r="F193" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G193" t="n">
+      <x:c r="G193" t="str">
         <x:v>74.80</x:v>
       </x:c>
     </x:row>
@@ -4484,7 +4484,7 @@
       <x:c r="F194" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G194" t="n">
+      <x:c r="G194" t="str">
         <x:v>74.83</x:v>
       </x:c>
     </x:row>
@@ -4507,7 +4507,7 @@
       <x:c r="F195" t="n">
         <x:v>3500.000</x:v>
       </x:c>
-      <x:c r="G195" t="n">
+      <x:c r="G195" t="str">
         <x:v>84.37</x:v>
       </x:c>
     </x:row>
@@ -4530,7 +4530,7 @@
       <x:c r="F196" t="n">
         <x:v>3500.000</x:v>
       </x:c>
-      <x:c r="G196" t="n">
+      <x:c r="G196" t="str">
         <x:v>82.13</x:v>
       </x:c>
     </x:row>
@@ -4553,7 +4553,7 @@
       <x:c r="F197" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G197" t="n">
+      <x:c r="G197" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4576,7 +4576,7 @@
       <x:c r="F198" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G198" t="n">
+      <x:c r="G198" t="str">
         <x:v>77.72</x:v>
       </x:c>
     </x:row>
@@ -4599,7 +4599,7 @@
       <x:c r="F199" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G199" t="n">
+      <x:c r="G199" t="str">
         <x:v>54.95</x:v>
       </x:c>
     </x:row>
@@ -4622,7 +4622,7 @@
       <x:c r="F200" t="n">
         <x:v>4043.000</x:v>
       </x:c>
-      <x:c r="G200" t="n">
+      <x:c r="G200" t="str">
         <x:v>52.30</x:v>
       </x:c>
     </x:row>
@@ -4645,7 +4645,7 @@
       <x:c r="F201" t="n">
         <x:v>11850.000</x:v>
       </x:c>
-      <x:c r="G201" t="n">
+      <x:c r="G201" t="str">
         <x:v>58.90</x:v>
       </x:c>
     </x:row>
@@ -4668,7 +4668,7 @@
       <x:c r="F202" t="n">
         <x:v>11447.317</x:v>
       </x:c>
-      <x:c r="G202" t="n">
+      <x:c r="G202" t="str">
         <x:v>81.57</x:v>
       </x:c>
     </x:row>
@@ -4691,7 +4691,7 @@
       <x:c r="F203" t="n">
         <x:v>7159.229</x:v>
       </x:c>
-      <x:c r="G203" t="n">
+      <x:c r="G203" t="str">
         <x:v>93.37</x:v>
       </x:c>
     </x:row>
@@ -4714,7 +4714,7 @@
       <x:c r="F204" t="n">
         <x:v>18778.629</x:v>
       </x:c>
-      <x:c r="G204" t="n">
+      <x:c r="G204" t="str">
         <x:v>91.18</x:v>
       </x:c>
     </x:row>
@@ -4737,7 +4737,7 @@
       <x:c r="F205" t="n">
         <x:v>3100.000</x:v>
       </x:c>
-      <x:c r="G205" t="n">
+      <x:c r="G205" t="str">
         <x:v>78.00</x:v>
       </x:c>
     </x:row>
@@ -4760,7 +4760,7 @@
       <x:c r="F206" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G206" t="n">
+      <x:c r="G206" t="str">
         <x:v>79.68</x:v>
       </x:c>
     </x:row>
@@ -4783,7 +4783,7 @@
       <x:c r="F207" t="n">
         <x:v>4135.930</x:v>
       </x:c>
-      <x:c r="G207" t="n">
+      <x:c r="G207" t="str">
         <x:v>63.63</x:v>
       </x:c>
     </x:row>
@@ -4806,7 +4806,7 @@
       <x:c r="F208" t="n">
         <x:v>3606.000</x:v>
       </x:c>
-      <x:c r="G208" t="n">
+      <x:c r="G208" t="str">
         <x:v>75.05</x:v>
       </x:c>
     </x:row>
@@ -4829,7 +4829,7 @@
       <x:c r="F209" t="n">
         <x:v>11228.319</x:v>
       </x:c>
-      <x:c r="G209" t="n">
+      <x:c r="G209" t="str">
         <x:v>77.78</x:v>
       </x:c>
     </x:row>
@@ -4852,7 +4852,7 @@
       <x:c r="F210" t="n">
         <x:v>8266.000</x:v>
       </x:c>
-      <x:c r="G210" t="n">
+      <x:c r="G210" t="str">
         <x:v>79.33</x:v>
       </x:c>
     </x:row>
@@ -4875,7 +4875,7 @@
       <x:c r="F211" t="n">
         <x:v>9577.269</x:v>
       </x:c>
-      <x:c r="G211" t="n">
+      <x:c r="G211" t="str">
         <x:v>78.90</x:v>
       </x:c>
     </x:row>
@@ -4898,7 +4898,7 @@
       <x:c r="F212" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G212" t="n">
+      <x:c r="G212" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -4921,7 +4921,7 @@
       <x:c r="F213" t="n">
         <x:v>3032.809</x:v>
       </x:c>
-      <x:c r="G213" t="n">
+      <x:c r="G213" t="str">
         <x:v>48.28</x:v>
       </x:c>
     </x:row>
@@ -4944,7 +4944,7 @@
       <x:c r="F214" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G214" t="n">
+      <x:c r="G214" t="str">
         <x:v>57.85</x:v>
       </x:c>
     </x:row>
@@ -4967,7 +4967,7 @@
       <x:c r="F215" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G215" t="n">
+      <x:c r="G215" t="str">
         <x:v>50.33</x:v>
       </x:c>
     </x:row>
@@ -4990,7 +4990,7 @@
       <x:c r="F216" t="n">
         <x:v>7959.844</x:v>
       </x:c>
-      <x:c r="G216" t="n">
+      <x:c r="G216" t="str">
         <x:v>49.57</x:v>
       </x:c>
     </x:row>
@@ -5013,7 +5013,7 @@
       <x:c r="F217" t="n">
         <x:v>1876.448</x:v>
       </x:c>
-      <x:c r="G217" t="n">
+      <x:c r="G217" t="str">
         <x:v>55.58</x:v>
       </x:c>
     </x:row>
@@ -5036,7 +5036,7 @@
       <x:c r="F218" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G218" t="n">
+      <x:c r="G218" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5059,7 +5059,7 @@
       <x:c r="F219" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G219" t="n">
+      <x:c r="G219" t="str">
         <x:v>65.22</x:v>
       </x:c>
     </x:row>
@@ -5082,7 +5082,7 @@
       <x:c r="F220" t="n">
         <x:v>4067.961</x:v>
       </x:c>
-      <x:c r="G220" t="n">
+      <x:c r="G220" t="str">
         <x:v>71.78</x:v>
       </x:c>
     </x:row>
@@ -5105,7 +5105,7 @@
       <x:c r="F221" t="n">
         <x:v>8649.557</x:v>
       </x:c>
-      <x:c r="G221" t="n">
+      <x:c r="G221" t="str">
         <x:v>67.80</x:v>
       </x:c>
     </x:row>
@@ -5128,7 +5128,7 @@
       <x:c r="F222" t="n">
         <x:v>8649.557</x:v>
       </x:c>
-      <x:c r="G222" t="n">
+      <x:c r="G222" t="str">
         <x:v>70.63</x:v>
       </x:c>
     </x:row>
@@ -5151,7 +5151,7 @@
       <x:c r="F223" t="n">
         <x:v>23663.000</x:v>
       </x:c>
-      <x:c r="G223" t="n">
+      <x:c r="G223" t="str">
         <x:v>68.13</x:v>
       </x:c>
     </x:row>
@@ -5174,7 +5174,7 @@
       <x:c r="F224" t="n">
         <x:v>5779.193</x:v>
       </x:c>
-      <x:c r="G224" t="n">
+      <x:c r="G224" t="str">
         <x:v>77.42</x:v>
       </x:c>
     </x:row>
@@ -5197,7 +5197,7 @@
       <x:c r="F225" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G225" t="n">
+      <x:c r="G225" t="str">
         <x:v>67.45</x:v>
       </x:c>
     </x:row>
@@ -5220,7 +5220,7 @@
       <x:c r="F226" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G226" t="n">
+      <x:c r="G226" t="str">
         <x:v>70.32</x:v>
       </x:c>
     </x:row>
@@ -5243,7 +5243,7 @@
       <x:c r="F227" t="n">
         <x:v>1006.000</x:v>
       </x:c>
-      <x:c r="G227" t="n">
+      <x:c r="G227" t="str">
         <x:v>54.05</x:v>
       </x:c>
     </x:row>
@@ -5266,7 +5266,7 @@
       <x:c r="F228" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G228" t="n">
+      <x:c r="G228" t="str">
         <x:v>62.68</x:v>
       </x:c>
     </x:row>
@@ -5289,7 +5289,7 @@
       <x:c r="F229" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G229" t="n">
+      <x:c r="G229" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5312,7 +5312,7 @@
       <x:c r="F230" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G230" t="n">
+      <x:c r="G230" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5335,7 +5335,7 @@
       <x:c r="F231" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G231" t="n">
+      <x:c r="G231" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5358,7 +5358,7 @@
       <x:c r="F232" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G232" t="n">
+      <x:c r="G232" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5381,7 +5381,7 @@
       <x:c r="F233" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G233" t="n">
+      <x:c r="G233" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5404,7 +5404,7 @@
       <x:c r="F234" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G234" t="n">
+      <x:c r="G234" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5427,7 +5427,7 @@
       <x:c r="F235" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G235" t="n">
+      <x:c r="G235" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5450,7 +5450,7 @@
       <x:c r="F236" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G236" t="n">
+      <x:c r="G236" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5473,7 +5473,7 @@
       <x:c r="F237" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G237" t="n">
+      <x:c r="G237" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5496,7 +5496,7 @@
       <x:c r="F238" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G238" t="n">
+      <x:c r="G238" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5519,7 +5519,7 @@
       <x:c r="F239" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G239" t="n">
+      <x:c r="G239" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5542,7 +5542,7 @@
       <x:c r="F240" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G240" t="n">
+      <x:c r="G240" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5565,7 +5565,7 @@
       <x:c r="F241" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G241" t="n">
+      <x:c r="G241" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5588,7 +5588,7 @@
       <x:c r="F242" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G242" t="n">
+      <x:c r="G242" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5611,7 +5611,7 @@
       <x:c r="F243" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G243" t="n">
+      <x:c r="G243" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5634,7 +5634,7 @@
       <x:c r="F244" t="n">
         <x:v>1037.693</x:v>
       </x:c>
-      <x:c r="G244" t="n">
+      <x:c r="G244" t="str">
         <x:v>61.67</x:v>
       </x:c>
     </x:row>
@@ -5657,7 +5657,7 @@
       <x:c r="F245" t="n">
         <x:v>7243.000</x:v>
       </x:c>
-      <x:c r="G245" t="n">
+      <x:c r="G245" t="str">
         <x:v>77.87</x:v>
       </x:c>
     </x:row>
@@ -5680,7 +5680,7 @@
       <x:c r="F246" t="n">
         <x:v>13334.725</x:v>
       </x:c>
-      <x:c r="G246" t="n">
+      <x:c r="G246" t="str">
         <x:v>77.87</x:v>
       </x:c>
     </x:row>
@@ -5703,7 +5703,7 @@
       <x:c r="F247" t="n">
         <x:v>14867.031</x:v>
       </x:c>
-      <x:c r="G247" t="n">
+      <x:c r="G247" t="str">
         <x:v>90.17</x:v>
       </x:c>
     </x:row>
@@ -5726,7 +5726,7 @@
       <x:c r="F248" t="n">
         <x:v>3479.273</x:v>
       </x:c>
-      <x:c r="G248" t="n">
+      <x:c r="G248" t="str">
         <x:v>63.43</x:v>
       </x:c>
     </x:row>
@@ -5749,7 +5749,7 @@
       <x:c r="F249" t="n">
         <x:v>2807.996</x:v>
       </x:c>
-      <x:c r="G249" t="n">
+      <x:c r="G249" t="str">
         <x:v>92.03</x:v>
       </x:c>
     </x:row>
@@ -5772,7 +5772,7 @@
       <x:c r="F250" t="n">
         <x:v>1706.000</x:v>
       </x:c>
-      <x:c r="G250" t="n">
+      <x:c r="G250" t="str">
         <x:v>48.78</x:v>
       </x:c>
     </x:row>
@@ -5795,7 +5795,7 @@
       <x:c r="F251" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G251" t="n">
+      <x:c r="G251" t="str">
         <x:v>40.02</x:v>
       </x:c>
     </x:row>
@@ -5818,7 +5818,7 @@
       <x:c r="F252" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G252" t="n">
+      <x:c r="G252" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5841,7 +5841,7 @@
       <x:c r="F253" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G253" t="n">
+      <x:c r="G253" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5864,7 +5864,7 @@
       <x:c r="F254" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G254" t="n">
+      <x:c r="G254" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5887,7 +5887,7 @@
       <x:c r="F255" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G255" t="n">
+      <x:c r="G255" t="str">
         <x:v>33.33</x:v>
       </x:c>
     </x:row>
@@ -5910,7 +5910,7 @@
       <x:c r="F256" t="n">
         <x:v>2006.000</x:v>
       </x:c>
-      <x:c r="G256" t="n">
+      <x:c r="G256" t="str">
         <x:v>33.33</x:v>
       </x:c>
     </x:row>
@@ -5933,7 +5933,7 @@
       <x:c r="F257" t="n">
         <x:v>906.000</x:v>
       </x:c>
-      <x:c r="G257" t="n">
+      <x:c r="G257" t="str">
         <x:v>28.60</x:v>
       </x:c>
     </x:row>
@@ -5956,7 +5956,7 @@
       <x:c r="F258" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G258" t="n">
+      <x:c r="G258" t="str">
         <x:v>37.68</x:v>
       </x:c>
     </x:row>
@@ -5979,7 +5979,7 @@
       <x:c r="F259" t="n">
         <x:v>1556.000</x:v>
       </x:c>
-      <x:c r="G259" t="n">
+      <x:c r="G259" t="str">
         <x:v>54.53</x:v>
       </x:c>
     </x:row>
@@ -6002,7 +6002,7 @@
       <x:c r="F260" t="n">
         <x:v>1917.000</x:v>
       </x:c>
-      <x:c r="G260" t="n">
+      <x:c r="G260" t="str">
         <x:v>50.92</x:v>
       </x:c>
     </x:row>
@@ -6025,7 +6025,7 @@
       <x:c r="F261" t="n">
         <x:v>6726.984</x:v>
       </x:c>
-      <x:c r="G261" t="n">
+      <x:c r="G261" t="str">
         <x:v>61.32</x:v>
       </x:c>
     </x:row>
@@ -6048,7 +6048,7 @@
       <x:c r="F262" t="n">
         <x:v>3147.000</x:v>
       </x:c>
-      <x:c r="G262" t="n">
+      <x:c r="G262" t="str">
         <x:v>53.27</x:v>
       </x:c>
     </x:row>
@@ -6071,7 +6071,7 @@
       <x:c r="F263" t="n">
         <x:v>3518.192</x:v>
       </x:c>
-      <x:c r="G263" t="n">
+      <x:c r="G263" t="str">
         <x:v>55.25</x:v>
       </x:c>
     </x:row>
@@ -6094,7 +6094,7 @@
       <x:c r="F264" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G264" t="n">
+      <x:c r="G264" t="str">
         <x:v>53.37</x:v>
       </x:c>
     </x:row>
@@ -6117,7 +6117,7 @@
       <x:c r="F265" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G265" t="n">
+      <x:c r="G265" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6140,7 +6140,7 @@
       <x:c r="F266" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G266" t="n">
+      <x:c r="G266" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6163,7 +6163,7 @@
       <x:c r="F267" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G267" t="n">
+      <x:c r="G267" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6186,7 +6186,7 @@
       <x:c r="F268" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G268" t="n">
+      <x:c r="G268" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6209,7 +6209,7 @@
       <x:c r="F269" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G269" t="n">
+      <x:c r="G269" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6232,7 +6232,7 @@
       <x:c r="F270" t="n">
         <x:v>2350.000</x:v>
       </x:c>
-      <x:c r="G270" t="n">
+      <x:c r="G270" t="str">
         <x:v>94.37</x:v>
       </x:c>
     </x:row>
@@ -6255,7 +6255,7 @@
       <x:c r="F271" t="n">
         <x:v>2350.000</x:v>
       </x:c>
-      <x:c r="G271" t="n">
+      <x:c r="G271" t="str">
         <x:v>94.37</x:v>
       </x:c>
     </x:row>
@@ -6278,7 +6278,7 @@
       <x:c r="F272" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G272" t="n">
+      <x:c r="G272" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6301,7 +6301,7 @@
       <x:c r="F273" t="n">
         <x:v>3956.000</x:v>
       </x:c>
-      <x:c r="G273" t="n">
+      <x:c r="G273" t="str">
         <x:v>65.27</x:v>
       </x:c>
     </x:row>
@@ -6324,7 +6324,7 @@
       <x:c r="F274" t="n">
         <x:v>1600.000</x:v>
       </x:c>
-      <x:c r="G274" t="n">
+      <x:c r="G274" t="str">
         <x:v>88.10</x:v>
       </x:c>
     </x:row>
@@ -6347,7 +6347,7 @@
       <x:c r="F275" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G275" t="n">
+      <x:c r="G275" t="str">
         <x:v>81.20</x:v>
       </x:c>
     </x:row>
@@ -6370,7 +6370,7 @@
       <x:c r="F276" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G276" t="n">
+      <x:c r="G276" t="str">
         <x:v>66.37</x:v>
       </x:c>
     </x:row>
@@ -6393,7 +6393,7 @@
       <x:c r="F277" t="n">
         <x:v>2413.000</x:v>
       </x:c>
-      <x:c r="G277" t="n">
+      <x:c r="G277" t="str">
         <x:v>58.95</x:v>
       </x:c>
     </x:row>
@@ -6416,7 +6416,7 @@
       <x:c r="F278" t="n">
         <x:v>6102.344</x:v>
       </x:c>
-      <x:c r="G278" t="n">
+      <x:c r="G278" t="str">
         <x:v>60.93</x:v>
       </x:c>
     </x:row>
@@ -6439,7 +6439,7 @@
       <x:c r="F279" t="n">
         <x:v>3150.000</x:v>
       </x:c>
-      <x:c r="G279" t="n">
+      <x:c r="G279" t="str">
         <x:v>97.85</x:v>
       </x:c>
     </x:row>
@@ -6462,7 +6462,7 @@
       <x:c r="F280" t="n">
         <x:v>2870.619</x:v>
       </x:c>
-      <x:c r="G280" t="n">
+      <x:c r="G280" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -6485,7 +6485,7 @@
       <x:c r="F281" t="n">
         <x:v>3603.210</x:v>
       </x:c>
-      <x:c r="G281" t="n">
+      <x:c r="G281" t="str">
         <x:v>68.88</x:v>
       </x:c>
     </x:row>
@@ -6508,7 +6508,7 @@
       <x:c r="F282" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G282" t="n">
+      <x:c r="G282" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6531,7 +6531,7 @@
       <x:c r="F283" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G283" t="n">
+      <x:c r="G283" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6554,7 +6554,7 @@
       <x:c r="F284" t="n">
         <x:v>4953.210</x:v>
       </x:c>
-      <x:c r="G284" t="n">
+      <x:c r="G284" t="str">
         <x:v>65.77</x:v>
       </x:c>
     </x:row>
@@ -6577,7 +6577,7 @@
       <x:c r="F285" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G285" t="n">
+      <x:c r="G285" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6600,7 +6600,7 @@
       <x:c r="F286" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G286" t="n">
+      <x:c r="G286" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6623,7 +6623,7 @@
       <x:c r="F287" t="n">
         <x:v>3753.210</x:v>
       </x:c>
-      <x:c r="G287" t="n">
+      <x:c r="G287" t="str">
         <x:v>41.15</x:v>
       </x:c>
     </x:row>
@@ -6646,7 +6646,7 @@
       <x:c r="F288" t="n">
         <x:v>1700.000</x:v>
       </x:c>
-      <x:c r="G288" t="n">
+      <x:c r="G288" t="str">
         <x:v>64.83</x:v>
       </x:c>
     </x:row>
@@ -6669,7 +6669,7 @@
       <x:c r="F289" t="n">
         <x:v>1650.000</x:v>
       </x:c>
-      <x:c r="G289" t="n">
+      <x:c r="G289" t="str">
         <x:v>91.90</x:v>
       </x:c>
     </x:row>
@@ -6692,7 +6692,7 @@
       <x:c r="F290" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G290" t="n">
+      <x:c r="G290" t="str">
         <x:v>58.23</x:v>
       </x:c>
     </x:row>
@@ -6715,7 +6715,7 @@
       <x:c r="F291" t="n">
         <x:v>1750.000</x:v>
       </x:c>
-      <x:c r="G291" t="n">
+      <x:c r="G291" t="str">
         <x:v>84.00</x:v>
       </x:c>
     </x:row>
@@ -6738,7 +6738,7 @@
       <x:c r="F292" t="n">
         <x:v>2153.210</x:v>
       </x:c>
-      <x:c r="G292" t="n">
+      <x:c r="G292" t="str">
         <x:v>77.33</x:v>
       </x:c>
     </x:row>
@@ -6761,7 +6761,7 @@
       <x:c r="F293" t="n">
         <x:v>6600.000</x:v>
       </x:c>
-      <x:c r="G293" t="n">
+      <x:c r="G293" t="str">
         <x:v>73.52</x:v>
       </x:c>
     </x:row>
@@ -6784,7 +6784,7 @@
       <x:c r="F294" t="n">
         <x:v>1530.000</x:v>
       </x:c>
-      <x:c r="G294" t="n">
+      <x:c r="G294" t="str">
         <x:v>96.77</x:v>
       </x:c>
     </x:row>
@@ -6807,7 +6807,7 @@
       <x:c r="F295" t="n">
         <x:v>930.000</x:v>
       </x:c>
-      <x:c r="G295" t="n">
+      <x:c r="G295" t="str">
         <x:v>88.07</x:v>
       </x:c>
     </x:row>
@@ -6830,7 +6830,7 @@
       <x:c r="F296" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G296" t="n">
+      <x:c r="G296" t="str">
         <x:v>84.13</x:v>
       </x:c>
     </x:row>
@@ -6853,7 +6853,7 @@
       <x:c r="F297" t="n">
         <x:v>3560.000</x:v>
       </x:c>
-      <x:c r="G297" t="n">
+      <x:c r="G297" t="str">
         <x:v>80.90</x:v>
       </x:c>
     </x:row>
@@ -6876,7 +6876,7 @@
       <x:c r="F298" t="n">
         <x:v>2403.772</x:v>
       </x:c>
-      <x:c r="G298" t="n">
+      <x:c r="G298" t="str">
         <x:v>77.00</x:v>
       </x:c>
     </x:row>
@@ -6899,7 +6899,7 @@
       <x:c r="F299" t="n">
         <x:v>4394.246</x:v>
       </x:c>
-      <x:c r="G299" t="n">
+      <x:c r="G299" t="str">
         <x:v>77.00</x:v>
       </x:c>
     </x:row>
@@ -6922,7 +6922,7 @@
       <x:c r="F300" t="n">
         <x:v>3855.754</x:v>
       </x:c>
-      <x:c r="G300" t="n">
+      <x:c r="G300" t="str">
         <x:v>91.60</x:v>
       </x:c>
     </x:row>
@@ -6945,7 +6945,7 @@
       <x:c r="F301" t="n">
         <x:v>2800.000</x:v>
       </x:c>
-      <x:c r="G301" t="n">
+      <x:c r="G301" t="str">
         <x:v>73.27</x:v>
       </x:c>
     </x:row>
@@ -6968,7 +6968,7 @@
       <x:c r="F302" t="n">
         <x:v>3744.215</x:v>
       </x:c>
-      <x:c r="G302" t="n">
+      <x:c r="G302" t="str">
         <x:v>77.17</x:v>
       </x:c>
     </x:row>
@@ -6991,7 +6991,7 @@
       <x:c r="F303" t="n">
         <x:v>1687.000</x:v>
       </x:c>
-      <x:c r="G303" t="n">
+      <x:c r="G303" t="str">
         <x:v>84.73</x:v>
       </x:c>
     </x:row>
@@ -7014,7 +7014,7 @@
       <x:c r="F304" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G304" t="n">
+      <x:c r="G304" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -7037,7 +7037,7 @@
       <x:c r="F305" t="n">
         <x:v>8151.985</x:v>
       </x:c>
-      <x:c r="G305" t="n">
+      <x:c r="G305" t="str">
         <x:v>57.18</x:v>
       </x:c>
     </x:row>
@@ -7060,7 +7060,7 @@
       <x:c r="F306" t="n">
         <x:v>3475.911</x:v>
       </x:c>
-      <x:c r="G306" t="n">
+      <x:c r="G306" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7083,7 +7083,7 @@
       <x:c r="F307" t="n">
         <x:v>14620.000</x:v>
       </x:c>
-      <x:c r="G307" t="n">
+      <x:c r="G307" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -7106,7 +7106,7 @@
       <x:c r="F308" t="n">
         <x:v>2150.000</x:v>
       </x:c>
-      <x:c r="G308" t="n">
+      <x:c r="G308" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -7129,7 +7129,7 @@
       <x:c r="F309" t="n">
         <x:v>5101.000</x:v>
       </x:c>
-      <x:c r="G309" t="n">
+      <x:c r="G309" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -7152,7 +7152,7 @@
       <x:c r="F310" t="n">
         <x:v>6665.979</x:v>
       </x:c>
-      <x:c r="G310" t="n">
+      <x:c r="G310" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -7175,7 +7175,7 @@
       <x:c r="F311" t="n">
         <x:v>5305.587</x:v>
       </x:c>
-      <x:c r="G311" t="n">
+      <x:c r="G311" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -7198,7 +7198,7 @@
       <x:c r="F312" t="n">
         <x:v>5333.466</x:v>
       </x:c>
-      <x:c r="G312" t="n">
+      <x:c r="G312" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
@@ -7221,7 +7221,7 @@
       <x:c r="F313" t="n">
         <x:v>2787.000</x:v>
       </x:c>
-      <x:c r="G313" t="n">
+      <x:c r="G313" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
@@ -7244,7 +7244,7 @@
       <x:c r="F314" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G314" t="n">
+      <x:c r="G314" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -7267,7 +7267,7 @@
       <x:c r="F315" t="n">
         <x:v>4384.000</x:v>
       </x:c>
-      <x:c r="G315" t="n">
+      <x:c r="G315" t="str">
         <x:v>84.73</x:v>
       </x:c>
     </x:row>
@@ -7290,7 +7290,7 @@
       <x:c r="F316" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G316" t="n">
+      <x:c r="G316" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7313,7 +7313,7 @@
       <x:c r="F317" t="n">
         <x:v>8462.000</x:v>
       </x:c>
-      <x:c r="G317" t="n">
+      <x:c r="G317" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7336,7 +7336,7 @@
       <x:c r="F318" t="n">
         <x:v>8196.993</x:v>
       </x:c>
-      <x:c r="G318" t="n">
+      <x:c r="G318" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7359,7 +7359,7 @@
       <x:c r="F319" t="n">
         <x:v>6511.970</x:v>
       </x:c>
-      <x:c r="G319" t="n">
+      <x:c r="G319" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7382,13 +7382,13 @@
       <x:c r="F320" t="n">
         <x:v>6997.239</x:v>
       </x:c>
-      <x:c r="G320" t="n">
+      <x:c r="G320" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:tableParts>
-    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc0765e58034e49a7"/>
+    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R44510aa9eabf489f"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Added cables count to the export table
</commit_message>
<xml_diff>
--- a/TraysFastUpdate/wwwroot/Trays.xlsx
+++ b/TraysFastUpdate/wwwroot/Trays.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trays" sheetId="1" r:id="R00e26a0dcbfe4fbe"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trays" sheetId="1" r:id="Rf10bc3a73ae74ba3"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Trays" displayName="Trays" ref="A1:G320">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Trays" displayName="Trays" ref="A1:H320">
   <x:autoFilter ref="A1:G320"/>
-  <x:tableColumns count="7">
+  <x:tableColumns count="8">
     <x:tableColumn id="1" name="Name"/>
     <x:tableColumn id="2" name="Type"/>
     <x:tableColumn id="3" name="Purpose"/>
     <x:tableColumn id="4" name="Width [mm]"/>
     <x:tableColumn id="5" name="Height [mm]"/>
     <x:tableColumn id="6" name="Length [mm]"/>
+    <x:tableColumn id="7" name="Cables on tray [pcs.]"/>
     <x:tableColumn id="8" name="Available space [%]"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -46,6 +47,9 @@
         <x:v>Length [mm]</x:v>
       </x:c>
       <x:c r="G1" t="str">
+        <x:v>Cables on tray [pcs.]</x:v>
+      </x:c>
+      <x:c r="H1" t="str">
         <x:v>Available space [%]</x:v>
       </x:c>
     </x:row>
@@ -60,7 +64,7 @@
         <x:v>Type B (Green color) for LV cables</x:v>
       </x:c>
       <x:c r="D2" t="n">
-        <x:v>300</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="E2" t="n">
         <x:v>100</x:v>
@@ -68,8 +72,11 @@
       <x:c r="F2" t="n">
         <x:v>7838.070</x:v>
       </x:c>
-      <x:c r="G2" t="str">
-        <x:v>75.67</x:v>
+      <x:c r="G2" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H2" t="str">
+        <x:v>51.33</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
@@ -91,7 +98,10 @@
       <x:c r="F3" t="n">
         <x:v>23600.619</x:v>
       </x:c>
-      <x:c r="G3" t="str">
+      <x:c r="G3" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H3" t="str">
         <x:v>63.60</x:v>
       </x:c>
     </x:row>
@@ -114,7 +124,10 @@
       <x:c r="F4" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G4" t="str">
+      <x:c r="G4" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H4" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -137,7 +150,10 @@
       <x:c r="F5" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G5" t="str">
+      <x:c r="G5" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H5" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -160,7 +176,10 @@
       <x:c r="F6" t="n">
         <x:v>1700.619</x:v>
       </x:c>
-      <x:c r="G6" t="str">
+      <x:c r="G6" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H6" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -183,7 +202,10 @@
       <x:c r="F7" t="n">
         <x:v>1700.619</x:v>
       </x:c>
-      <x:c r="G7" t="str">
+      <x:c r="G7" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H7" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -206,7 +228,10 @@
       <x:c r="F8" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G8" t="str">
+      <x:c r="G8" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H8" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -229,7 +254,10 @@
       <x:c r="F9" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G9" t="str">
+      <x:c r="G9" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H9" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -252,7 +280,10 @@
       <x:c r="F10" t="n">
         <x:v>6325.284</x:v>
       </x:c>
-      <x:c r="G10" t="str">
+      <x:c r="G10" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H10" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -275,7 +306,10 @@
       <x:c r="F11" t="n">
         <x:v>6325.284</x:v>
       </x:c>
-      <x:c r="G11" t="str">
+      <x:c r="G11" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H11" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -298,7 +332,10 @@
       <x:c r="F12" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G12" t="str">
+      <x:c r="G12" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H12" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -321,7 +358,10 @@
       <x:c r="F13" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G13" t="str">
+      <x:c r="G13" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H13" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -344,7 +384,10 @@
       <x:c r="F14" t="n">
         <x:v>5764.057</x:v>
       </x:c>
-      <x:c r="G14" t="str">
+      <x:c r="G14" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H14" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -367,7 +410,10 @@
       <x:c r="F15" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G15" t="str">
+      <x:c r="G15" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H15" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -390,7 +436,10 @@
       <x:c r="F16" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G16" t="str">
+      <x:c r="G16" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H16" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -413,7 +462,10 @@
       <x:c r="F17" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G17" t="str">
+      <x:c r="G17" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H17" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -436,7 +488,10 @@
       <x:c r="F18" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G18" t="str">
+      <x:c r="G18" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H18" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -459,7 +514,10 @@
       <x:c r="F19" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G19" t="str">
+      <x:c r="G19" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H19" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -482,7 +540,10 @@
       <x:c r="F20" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G20" t="str">
+      <x:c r="G20" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H20" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -505,7 +566,10 @@
       <x:c r="F21" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G21" t="str">
+      <x:c r="G21" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H21" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -528,7 +592,10 @@
       <x:c r="F22" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G22" t="str">
+      <x:c r="G22" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H22" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -551,7 +618,10 @@
       <x:c r="F23" t="n">
         <x:v>11439.220</x:v>
       </x:c>
-      <x:c r="G23" t="str">
+      <x:c r="G23" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H23" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -574,7 +644,10 @@
       <x:c r="F24" t="n">
         <x:v>11439.220</x:v>
       </x:c>
-      <x:c r="G24" t="str">
+      <x:c r="G24" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H24" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -597,7 +670,10 @@
       <x:c r="F25" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G25" t="str">
+      <x:c r="G25" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H25" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -620,7 +696,10 @@
       <x:c r="F26" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G26" t="str">
+      <x:c r="G26" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H26" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -643,7 +722,10 @@
       <x:c r="F27" t="n">
         <x:v>5642.599</x:v>
       </x:c>
-      <x:c r="G27" t="str">
+      <x:c r="G27" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H27" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -666,7 +748,10 @@
       <x:c r="F28" t="n">
         <x:v>5643.821</x:v>
       </x:c>
-      <x:c r="G28" t="str">
+      <x:c r="G28" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H28" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -689,7 +774,10 @@
       <x:c r="F29" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G29" t="str">
+      <x:c r="G29" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H29" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -712,7 +800,10 @@
       <x:c r="F30" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G30" t="str">
+      <x:c r="G30" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H30" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -735,7 +826,10 @@
       <x:c r="F31" t="n">
         <x:v>1800.000</x:v>
       </x:c>
-      <x:c r="G31" t="str">
+      <x:c r="G31" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H31" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -758,7 +852,10 @@
       <x:c r="F32" t="n">
         <x:v>1800.000</x:v>
       </x:c>
-      <x:c r="G32" t="str">
+      <x:c r="G32" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H32" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -781,7 +878,10 @@
       <x:c r="F33" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G33" t="str">
+      <x:c r="G33" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H33" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -804,7 +904,10 @@
       <x:c r="F34" t="n">
         <x:v>1274.601</x:v>
       </x:c>
-      <x:c r="G34" t="str">
+      <x:c r="G34" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H34" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -827,7 +930,10 @@
       <x:c r="F35" t="n">
         <x:v>5830.812</x:v>
       </x:c>
-      <x:c r="G35" t="str">
+      <x:c r="G35" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H35" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -850,7 +956,10 @@
       <x:c r="F36" t="n">
         <x:v>5830.812</x:v>
       </x:c>
-      <x:c r="G36" t="str">
+      <x:c r="G36" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H36" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -873,7 +982,10 @@
       <x:c r="F37" t="n">
         <x:v>4970.900</x:v>
       </x:c>
-      <x:c r="G37" t="str">
+      <x:c r="G37" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H37" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -896,7 +1008,10 @@
       <x:c r="F38" t="n">
         <x:v>11174.950</x:v>
       </x:c>
-      <x:c r="G38" t="str">
+      <x:c r="G38" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H38" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -919,7 +1034,10 @@
       <x:c r="F39" t="n">
         <x:v>10327.774</x:v>
       </x:c>
-      <x:c r="G39" t="str">
+      <x:c r="G39" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H39" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -942,7 +1060,10 @@
       <x:c r="F40" t="n">
         <x:v>25905.369</x:v>
       </x:c>
-      <x:c r="G40" t="str">
+      <x:c r="G40" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H40" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -965,7 +1086,10 @@
       <x:c r="F41" t="n">
         <x:v>25105.369</x:v>
       </x:c>
-      <x:c r="G41" t="str">
+      <x:c r="G41" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H41" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -988,7 +1112,10 @@
       <x:c r="F42" t="n">
         <x:v>10326.481</x:v>
       </x:c>
-      <x:c r="G42" t="str">
+      <x:c r="G42" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H42" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1011,7 +1138,10 @@
       <x:c r="F43" t="n">
         <x:v>11174.424</x:v>
       </x:c>
-      <x:c r="G43" t="str">
+      <x:c r="G43" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H43" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1034,7 +1164,10 @@
       <x:c r="F44" t="n">
         <x:v>4218.868</x:v>
       </x:c>
-      <x:c r="G44" t="str">
+      <x:c r="G44" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H44" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1057,7 +1190,10 @@
       <x:c r="F45" t="n">
         <x:v>5764.057</x:v>
       </x:c>
-      <x:c r="G45" t="str">
+      <x:c r="G45" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H45" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1080,7 +1216,10 @@
       <x:c r="F46" t="n">
         <x:v>5642.620</x:v>
       </x:c>
-      <x:c r="G46" t="str">
+      <x:c r="G46" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H46" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1103,7 +1242,10 @@
       <x:c r="F47" t="n">
         <x:v>5642.620</x:v>
       </x:c>
-      <x:c r="G47" t="str">
+      <x:c r="G47" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H47" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1126,7 +1268,10 @@
       <x:c r="F48" t="n">
         <x:v>7736.447</x:v>
       </x:c>
-      <x:c r="G48" t="str">
+      <x:c r="G48" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H48" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1149,7 +1294,10 @@
       <x:c r="F49" t="n">
         <x:v>7736.447</x:v>
       </x:c>
-      <x:c r="G49" t="str">
+      <x:c r="G49" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H49" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1172,7 +1320,10 @@
       <x:c r="F50" t="n">
         <x:v>10433.601</x:v>
       </x:c>
-      <x:c r="G50" t="str">
+      <x:c r="G50" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H50" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1195,7 +1346,10 @@
       <x:c r="F51" t="n">
         <x:v>10433.601</x:v>
       </x:c>
-      <x:c r="G51" t="str">
+      <x:c r="G51" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H51" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1218,7 +1372,10 @@
       <x:c r="F52" t="n">
         <x:v>6912.929</x:v>
       </x:c>
-      <x:c r="G52" t="str">
+      <x:c r="G52" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H52" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1241,7 +1398,10 @@
       <x:c r="F53" t="n">
         <x:v>7062.451</x:v>
       </x:c>
-      <x:c r="G53" t="str">
+      <x:c r="G53" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H53" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1264,7 +1424,10 @@
       <x:c r="F54" t="n">
         <x:v>6912.929</x:v>
       </x:c>
-      <x:c r="G54" t="str">
+      <x:c r="G54" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H54" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1287,7 +1450,10 @@
       <x:c r="F55" t="n">
         <x:v>6968.311</x:v>
       </x:c>
-      <x:c r="G55" t="str">
+      <x:c r="G55" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H55" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1310,7 +1476,10 @@
       <x:c r="F56" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G56" t="str">
+      <x:c r="G56" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H56" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1333,7 +1502,10 @@
       <x:c r="F57" t="n">
         <x:v>4725.000</x:v>
       </x:c>
-      <x:c r="G57" t="str">
+      <x:c r="G57" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H57" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1356,7 +1528,10 @@
       <x:c r="F58" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G58" t="str">
+      <x:c r="G58" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H58" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1379,7 +1554,10 @@
       <x:c r="F59" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G59" t="str">
+      <x:c r="G59" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H59" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1402,7 +1580,10 @@
       <x:c r="F60" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G60" t="str">
+      <x:c r="G60" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H60" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1425,7 +1606,10 @@
       <x:c r="F61" t="n">
         <x:v>5025.000</x:v>
       </x:c>
-      <x:c r="G61" t="str">
+      <x:c r="G61" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H61" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1448,7 +1632,10 @@
       <x:c r="F62" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G62" t="str">
+      <x:c r="G62" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H62" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1471,7 +1658,10 @@
       <x:c r="F63" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G63" t="str">
+      <x:c r="G63" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H63" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1494,7 +1684,10 @@
       <x:c r="F64" t="n">
         <x:v>6894.960</x:v>
       </x:c>
-      <x:c r="G64" t="str">
+      <x:c r="G64" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H64" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1517,7 +1710,10 @@
       <x:c r="F65" t="n">
         <x:v>7084.929</x:v>
       </x:c>
-      <x:c r="G65" t="str">
+      <x:c r="G65" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H65" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1540,7 +1736,10 @@
       <x:c r="F66" t="n">
         <x:v>6962.449</x:v>
       </x:c>
-      <x:c r="G66" t="str">
+      <x:c r="G66" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H66" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1563,7 +1762,10 @@
       <x:c r="F67" t="n">
         <x:v>7084.929</x:v>
       </x:c>
-      <x:c r="G67" t="str">
+      <x:c r="G67" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H67" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1586,7 +1788,10 @@
       <x:c r="F68" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G68" t="str">
+      <x:c r="G68" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H68" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1609,7 +1814,10 @@
       <x:c r="F69" t="n">
         <x:v>5025.000</x:v>
       </x:c>
-      <x:c r="G69" t="str">
+      <x:c r="G69" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H69" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1632,7 +1840,10 @@
       <x:c r="F70" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G70" t="str">
+      <x:c r="G70" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H70" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1655,7 +1866,10 @@
       <x:c r="F71" t="n">
         <x:v>3600.000</x:v>
       </x:c>
-      <x:c r="G71" t="str">
+      <x:c r="G71" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H71" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1678,7 +1892,10 @@
       <x:c r="F72" t="n">
         <x:v>5725.000</x:v>
       </x:c>
-      <x:c r="G72" t="str">
+      <x:c r="G72" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H72" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1701,7 +1918,10 @@
       <x:c r="F73" t="n">
         <x:v>5125.000</x:v>
       </x:c>
-      <x:c r="G73" t="str">
+      <x:c r="G73" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H73" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1724,7 +1944,10 @@
       <x:c r="F74" t="n">
         <x:v>2700.000</x:v>
       </x:c>
-      <x:c r="G74" t="str">
+      <x:c r="G74" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H74" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1747,7 +1970,10 @@
       <x:c r="F75" t="n">
         <x:v>2700.000</x:v>
       </x:c>
-      <x:c r="G75" t="str">
+      <x:c r="G75" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H75" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1770,7 +1996,10 @@
       <x:c r="F76" t="n">
         <x:v>21256.580</x:v>
       </x:c>
-      <x:c r="G76" t="str">
+      <x:c r="G76" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H76" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1793,7 +2022,10 @@
       <x:c r="F77" t="n">
         <x:v>20637.837</x:v>
       </x:c>
-      <x:c r="G77" t="str">
+      <x:c r="G77" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H77" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1816,7 +2048,10 @@
       <x:c r="F78" t="n">
         <x:v>22200.718</x:v>
       </x:c>
-      <x:c r="G78" t="str">
+      <x:c r="G78" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H78" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1839,7 +2074,10 @@
       <x:c r="F79" t="n">
         <x:v>21286.580</x:v>
       </x:c>
-      <x:c r="G79" t="str">
+      <x:c r="G79" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H79" t="str">
         <x:v>N/A</x:v>
       </x:c>
     </x:row>
@@ -1862,7 +2100,10 @@
       <x:c r="F80" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G80" t="str">
+      <x:c r="G80" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="H80" t="str">
         <x:v>38.65</x:v>
       </x:c>
     </x:row>
@@ -1885,7 +2126,10 @@
       <x:c r="F81" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G81" t="str">
+      <x:c r="G81" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H81" t="str">
         <x:v>63.47</x:v>
       </x:c>
     </x:row>
@@ -1908,7 +2152,10 @@
       <x:c r="F82" t="n">
         <x:v>7159.229</x:v>
       </x:c>
-      <x:c r="G82" t="str">
+      <x:c r="G82" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H82" t="str">
         <x:v>72.53</x:v>
       </x:c>
     </x:row>
@@ -1931,7 +2178,10 @@
       <x:c r="F83" t="n">
         <x:v>3250.000</x:v>
       </x:c>
-      <x:c r="G83" t="str">
+      <x:c r="G83" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H83" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
@@ -1954,13 +2204,16 @@
       <x:c r="F84" t="n">
         <x:v>1900.000</x:v>
       </x:c>
-      <x:c r="G84" t="str">
+      <x:c r="G84" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H84" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
     <x:row r="85">
       <x:c r="A85" t="str">
-        <x:v>B007</x:v>
+        <x:v>B101</x:v>
       </x:c>
       <x:c r="B85" t="str">
         <x:v>KL 100.603 F</x:v>
@@ -1975,18 +2228,21 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F85" t="n">
-        <x:v>6000.000</x:v>
-      </x:c>
-      <x:c r="G85" t="str">
-        <x:v>100.00</x:v>
+        <x:v>3606.000</x:v>
+      </x:c>
+      <x:c r="G85" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="H85" t="str">
+        <x:v>34.87</x:v>
       </x:c>
     </x:row>
     <x:row r="86">
       <x:c r="A86" t="str">
-        <x:v>B101</x:v>
+        <x:v>B102</x:v>
       </x:c>
       <x:c r="B86" t="str">
-        <x:v>KL 100.603 F</x:v>
+        <x:v>WSL 105.600 F</x:v>
       </x:c>
       <x:c r="C86" t="str">
         <x:v>Type B (Green color) for LV cables</x:v>
@@ -1995,21 +2251,24 @@
         <x:v>600</x:v>
       </x:c>
       <x:c r="E86" t="n">
-        <x:v>100</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="F86" t="n">
-        <x:v>3606.000</x:v>
-      </x:c>
-      <x:c r="G86" t="str">
-        <x:v>34.87</x:v>
+        <x:v>8778.319</x:v>
+      </x:c>
+      <x:c r="G86" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H86" t="str">
+        <x:v>67.07</x:v>
       </x:c>
     </x:row>
     <x:row r="87">
       <x:c r="A87" t="str">
-        <x:v>B102</x:v>
+        <x:v>B107-1</x:v>
       </x:c>
       <x:c r="B87" t="str">
-        <x:v>WSL 105.600 F</x:v>
+        <x:v>KL 100.603 F</x:v>
       </x:c>
       <x:c r="C87" t="str">
         <x:v>Type B (Green color) for LV cables</x:v>
@@ -2018,13 +2277,16 @@
         <x:v>600</x:v>
       </x:c>
       <x:c r="E87" t="n">
-        <x:v>105</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F87" t="n">
-        <x:v>8778.319</x:v>
-      </x:c>
-      <x:c r="G87" t="str">
-        <x:v>67.07</x:v>
+        <x:v>3032.809</x:v>
+      </x:c>
+      <x:c r="G87" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="H87" t="str">
+        <x:v>37.40</x:v>
       </x:c>
     </x:row>
     <x:row r="88">
@@ -2038,7 +2300,7 @@
         <x:v>Type B (Green color) for LV cables</x:v>
       </x:c>
       <x:c r="D88" t="n">
-        <x:v>600</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="E88" t="n">
         <x:v>100</x:v>
@@ -2046,13 +2308,16 @@
       <x:c r="F88" t="n">
         <x:v>1300.619</x:v>
       </x:c>
-      <x:c r="G88" t="str">
+      <x:c r="G88" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H88" t="str">
         <x:v>89.85</x:v>
       </x:c>
     </x:row>
     <x:row r="89">
       <x:c r="A89" t="str">
-        <x:v>B107-1</x:v>
+        <x:v>B105-1</x:v>
       </x:c>
       <x:c r="B89" t="str">
         <x:v>KL 100.603 F</x:v>
@@ -2061,21 +2326,24 @@
         <x:v>Type B (Green color) for LV cables</x:v>
       </x:c>
       <x:c r="D89" t="n">
-        <x:v>600</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="E89" t="n">
         <x:v>100</x:v>
       </x:c>
       <x:c r="F89" t="n">
-        <x:v>3032.809</x:v>
-      </x:c>
-      <x:c r="G89" t="str">
-        <x:v>37.40</x:v>
+        <x:v>6501.881</x:v>
+      </x:c>
+      <x:c r="G89" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H89" t="str">
+        <x:v>51.33</x:v>
       </x:c>
     </x:row>
     <x:row r="90">
       <x:c r="A90" t="str">
-        <x:v>B105-1</x:v>
+        <x:v>B105-2</x:v>
       </x:c>
       <x:c r="B90" t="str">
         <x:v>KL 100.603 F</x:v>
@@ -2090,15 +2358,18 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F90" t="n">
-        <x:v>6501.881</x:v>
-      </x:c>
-      <x:c r="G90" t="str">
-        <x:v>51.33</x:v>
+        <x:v>1196.290</x:v>
+      </x:c>
+      <x:c r="G90" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H90" t="str">
+        <x:v>43.13</x:v>
       </x:c>
     </x:row>
     <x:row r="91">
       <x:c r="A91" t="str">
-        <x:v>B105-2</x:v>
+        <x:v>B105-3</x:v>
       </x:c>
       <x:c r="B91" t="str">
         <x:v>KL 100.603 F</x:v>
@@ -2113,15 +2384,18 @@
         <x:v>100</x:v>
       </x:c>
       <x:c r="F91" t="n">
-        <x:v>1196.290</x:v>
-      </x:c>
-      <x:c r="G91" t="str">
-        <x:v>43.13</x:v>
+        <x:v>1879.028</x:v>
+      </x:c>
+      <x:c r="G91" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H91" t="str">
+        <x:v>67.95</x:v>
       </x:c>
     </x:row>
     <x:row r="92">
       <x:c r="A92" t="str">
-        <x:v>B105-3</x:v>
+        <x:v>B007</x:v>
       </x:c>
       <x:c r="B92" t="str">
         <x:v>KL 100.603 F</x:v>
@@ -2130,16 +2404,19 @@
         <x:v>Type B (Green color) for LV cables</x:v>
       </x:c>
       <x:c r="D92" t="n">
-        <x:v>400</x:v>
+        <x:v>600</x:v>
       </x:c>
       <x:c r="E92" t="n">
         <x:v>100</x:v>
       </x:c>
       <x:c r="F92" t="n">
-        <x:v>1879.028</x:v>
-      </x:c>
-      <x:c r="G92" t="str">
-        <x:v>67.95</x:v>
+        <x:v>6000.000</x:v>
+      </x:c>
+      <x:c r="G92" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H92" t="str">
+        <x:v>100.00</x:v>
       </x:c>
     </x:row>
     <x:row r="93">
@@ -2161,7 +2438,10 @@
       <x:c r="F93" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G93" t="str">
+      <x:c r="G93" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H93" t="str">
         <x:v>49.80</x:v>
       </x:c>
     </x:row>
@@ -2184,7 +2464,10 @@
       <x:c r="F94" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G94" t="str">
+      <x:c r="G94" t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="H94" t="str">
         <x:v>57.73</x:v>
       </x:c>
     </x:row>
@@ -2207,7 +2490,10 @@
       <x:c r="F95" t="n">
         <x:v>7909.844</x:v>
       </x:c>
-      <x:c r="G95" t="str">
+      <x:c r="G95" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H95" t="str">
         <x:v>62.22</x:v>
       </x:c>
     </x:row>
@@ -2230,7 +2516,10 @@
       <x:c r="F96" t="n">
         <x:v>1926.448</x:v>
       </x:c>
-      <x:c r="G96" t="str">
+      <x:c r="G96" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="H96" t="str">
         <x:v>72.32</x:v>
       </x:c>
     </x:row>
@@ -2253,7 +2542,10 @@
       <x:c r="F97" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G97" t="str">
+      <x:c r="G97" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H97" t="str">
         <x:v>72.32</x:v>
       </x:c>
     </x:row>
@@ -2276,7 +2568,10 @@
       <x:c r="F98" t="n">
         <x:v>4872.000</x:v>
       </x:c>
-      <x:c r="G98" t="str">
+      <x:c r="G98" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H98" t="str">
         <x:v>76.80</x:v>
       </x:c>
     </x:row>
@@ -2299,7 +2594,10 @@
       <x:c r="F99" t="n">
         <x:v>9001.937</x:v>
       </x:c>
-      <x:c r="G99" t="str">
+      <x:c r="G99" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H99" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2322,7 +2620,10 @@
       <x:c r="F100" t="n">
         <x:v>8951.937</x:v>
       </x:c>
-      <x:c r="G100" t="str">
+      <x:c r="G100" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H100" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2345,7 +2646,10 @@
       <x:c r="F101" t="n">
         <x:v>7926.000</x:v>
       </x:c>
-      <x:c r="G101" t="str">
+      <x:c r="G101" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H101" t="str">
         <x:v>81.80</x:v>
       </x:c>
     </x:row>
@@ -2368,7 +2672,10 @@
       <x:c r="F102" t="n">
         <x:v>12000.000</x:v>
       </x:c>
-      <x:c r="G102" t="str">
+      <x:c r="G102" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H102" t="str">
         <x:v>75.05</x:v>
       </x:c>
     </x:row>
@@ -2391,7 +2698,10 @@
       <x:c r="F103" t="n">
         <x:v>5638.090</x:v>
       </x:c>
-      <x:c r="G103" t="str">
+      <x:c r="G103" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H103" t="str">
         <x:v>82.33</x:v>
       </x:c>
     </x:row>
@@ -2414,7 +2724,10 @@
       <x:c r="F104" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G104" t="str">
+      <x:c r="G104" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H104" t="str">
         <x:v>73.42</x:v>
       </x:c>
     </x:row>
@@ -2437,7 +2750,10 @@
       <x:c r="F105" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G105" t="str">
+      <x:c r="G105" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H105" t="str">
         <x:v>76.97</x:v>
       </x:c>
     </x:row>
@@ -2460,7 +2776,10 @@
       <x:c r="F106" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G106" t="str">
+      <x:c r="G106" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H106" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2483,7 +2802,10 @@
       <x:c r="F107" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G107" t="str">
+      <x:c r="G107" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H107" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2506,7 +2828,10 @@
       <x:c r="F108" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G108" t="str">
+      <x:c r="G108" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H108" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2529,7 +2854,10 @@
       <x:c r="F109" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G109" t="str">
+      <x:c r="G109" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H109" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2552,7 +2880,10 @@
       <x:c r="F110" t="n">
         <x:v>10013.554</x:v>
       </x:c>
-      <x:c r="G110" t="str">
+      <x:c r="G110" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H110" t="str">
         <x:v>72.70</x:v>
       </x:c>
     </x:row>
@@ -2575,7 +2906,10 @@
       <x:c r="F111" t="n">
         <x:v>4251.206</x:v>
       </x:c>
-      <x:c r="G111" t="str">
+      <x:c r="G111" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H111" t="str">
         <x:v>57.27</x:v>
       </x:c>
     </x:row>
@@ -2598,7 +2932,10 @@
       <x:c r="F112" t="n">
         <x:v>12056.603</x:v>
       </x:c>
-      <x:c r="G112" t="str">
+      <x:c r="G112" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H112" t="str">
         <x:v>76.25</x:v>
       </x:c>
     </x:row>
@@ -2621,7 +2958,10 @@
       <x:c r="F113" t="n">
         <x:v>3706.090</x:v>
       </x:c>
-      <x:c r="G113" t="str">
+      <x:c r="G113" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H113" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2644,7 +2984,10 @@
       <x:c r="F114" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G114" t="str">
+      <x:c r="G114" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H114" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2667,7 +3010,10 @@
       <x:c r="F115" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G115" t="str">
+      <x:c r="G115" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H115" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2690,7 +3036,10 @@
       <x:c r="F116" t="n">
         <x:v>7909.844</x:v>
       </x:c>
-      <x:c r="G116" t="str">
+      <x:c r="G116" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H116" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2713,7 +3062,10 @@
       <x:c r="F117" t="n">
         <x:v>1926.448</x:v>
       </x:c>
-      <x:c r="G117" t="str">
+      <x:c r="G117" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H117" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2736,7 +3088,10 @@
       <x:c r="F118" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G118" t="str">
+      <x:c r="G118" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H118" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -2759,7 +3114,10 @@
       <x:c r="F119" t="n">
         <x:v>4067.961</x:v>
       </x:c>
-      <x:c r="G119" t="str">
+      <x:c r="G119" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H119" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -2782,7 +3140,10 @@
       <x:c r="F120" t="n">
         <x:v>1537.693</x:v>
       </x:c>
-      <x:c r="G120" t="str">
+      <x:c r="G120" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H120" t="str">
         <x:v>60.58</x:v>
       </x:c>
     </x:row>
@@ -2805,7 +3166,10 @@
       <x:c r="F121" t="n">
         <x:v>6678.620</x:v>
       </x:c>
-      <x:c r="G121" t="str">
+      <x:c r="G121" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H121" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -2828,7 +3192,10 @@
       <x:c r="F122" t="n">
         <x:v>13117.566</x:v>
       </x:c>
-      <x:c r="G122" t="str">
+      <x:c r="G122" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H122" t="str">
         <x:v>57.13</x:v>
       </x:c>
     </x:row>
@@ -2851,7 +3218,10 @@
       <x:c r="F123" t="n">
         <x:v>14559.495</x:v>
       </x:c>
-      <x:c r="G123" t="str">
+      <x:c r="G123" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H123" t="str">
         <x:v>79.38</x:v>
       </x:c>
     </x:row>
@@ -2874,7 +3244,10 @@
       <x:c r="F124" t="n">
         <x:v>4919.273</x:v>
       </x:c>
-      <x:c r="G124" t="str">
+      <x:c r="G124" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H124" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2897,7 +3270,10 @@
       <x:c r="F125" t="n">
         <x:v>3890.930</x:v>
       </x:c>
-      <x:c r="G125" t="str">
+      <x:c r="G125" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H125" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2920,7 +3296,10 @@
       <x:c r="F126" t="n">
         <x:v>2807.996</x:v>
       </x:c>
-      <x:c r="G126" t="str">
+      <x:c r="G126" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H126" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -2943,7 +3322,10 @@
       <x:c r="F127" t="n">
         <x:v>4100.000</x:v>
       </x:c>
-      <x:c r="G127" t="str">
+      <x:c r="G127" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="H127" t="str">
         <x:v>61.80</x:v>
       </x:c>
     </x:row>
@@ -2966,7 +3348,10 @@
       <x:c r="F128" t="n">
         <x:v>6465.000</x:v>
       </x:c>
-      <x:c r="G128" t="str">
+      <x:c r="G128" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="H128" t="str">
         <x:v>59.37</x:v>
       </x:c>
     </x:row>
@@ -2989,7 +3374,10 @@
       <x:c r="F129" t="n">
         <x:v>9500.000</x:v>
       </x:c>
-      <x:c r="G129" t="str">
+      <x:c r="G129" t="n">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="H129" t="str">
         <x:v>57.40</x:v>
       </x:c>
     </x:row>
@@ -3012,7 +3400,10 @@
       <x:c r="F130" t="n">
         <x:v>4400.000</x:v>
       </x:c>
-      <x:c r="G130" t="str">
+      <x:c r="G130" t="n">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="H130" t="str">
         <x:v>57.40</x:v>
       </x:c>
     </x:row>
@@ -3035,7 +3426,10 @@
       <x:c r="F131" t="n">
         <x:v>4703.319</x:v>
       </x:c>
-      <x:c r="G131" t="str">
+      <x:c r="G131" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H131" t="str">
         <x:v>87.43</x:v>
       </x:c>
     </x:row>
@@ -3058,7 +3452,10 @@
       <x:c r="F132" t="n">
         <x:v>4375.000</x:v>
       </x:c>
-      <x:c r="G132" t="str">
+      <x:c r="G132" t="n">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="H132" t="str">
         <x:v>61.85</x:v>
       </x:c>
     </x:row>
@@ -3081,7 +3478,10 @@
       <x:c r="F133" t="n">
         <x:v>12016.902</x:v>
       </x:c>
-      <x:c r="G133" t="str">
+      <x:c r="G133" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H133" t="str">
         <x:v>93.30</x:v>
       </x:c>
     </x:row>
@@ -3104,7 +3504,10 @@
       <x:c r="F134" t="n">
         <x:v>6719.875</x:v>
       </x:c>
-      <x:c r="G134" t="str">
+      <x:c r="G134" t="n">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="H134" t="str">
         <x:v>64.70</x:v>
       </x:c>
     </x:row>
@@ -3127,7 +3530,10 @@
       <x:c r="F135" t="n">
         <x:v>2915.000</x:v>
       </x:c>
-      <x:c r="G135" t="str">
+      <x:c r="G135" t="n">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="H135" t="str">
         <x:v>64.70</x:v>
       </x:c>
     </x:row>
@@ -3150,7 +3556,10 @@
       <x:c r="F136" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G136" t="str">
+      <x:c r="G136" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="H136" t="str">
         <x:v>72.40</x:v>
       </x:c>
     </x:row>
@@ -3173,7 +3582,10 @@
       <x:c r="F137" t="n">
         <x:v>4157.061</x:v>
       </x:c>
-      <x:c r="G137" t="str">
+      <x:c r="G137" t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="H137" t="str">
         <x:v>77.20</x:v>
       </x:c>
     </x:row>
@@ -3196,7 +3608,10 @@
       <x:c r="F138" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G138" t="str">
+      <x:c r="G138" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H138" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3219,7 +3634,10 @@
       <x:c r="F139" t="n">
         <x:v>4768.319</x:v>
       </x:c>
-      <x:c r="G139" t="str">
+      <x:c r="G139" t="n">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="H139" t="str">
         <x:v>53.63</x:v>
       </x:c>
     </x:row>
@@ -3242,7 +3660,10 @@
       <x:c r="F140" t="n">
         <x:v>6897.001</x:v>
       </x:c>
-      <x:c r="G140" t="str">
+      <x:c r="G140" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H140" t="str">
         <x:v>76.17</x:v>
       </x:c>
     </x:row>
@@ -3265,7 +3686,10 @@
       <x:c r="F141" t="n">
         <x:v>6897.001</x:v>
       </x:c>
-      <x:c r="G141" t="str">
+      <x:c r="G141" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H141" t="str">
         <x:v>76.17</x:v>
       </x:c>
     </x:row>
@@ -3288,7 +3712,10 @@
       <x:c r="F142" t="n">
         <x:v>5709.616</x:v>
       </x:c>
-      <x:c r="G142" t="str">
+      <x:c r="G142" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H142" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3311,7 +3738,10 @@
       <x:c r="F143" t="n">
         <x:v>4953.004</x:v>
       </x:c>
-      <x:c r="G143" t="str">
+      <x:c r="G143" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H143" t="str">
         <x:v>70.90</x:v>
       </x:c>
     </x:row>
@@ -3334,7 +3764,10 @@
       <x:c r="F144" t="n">
         <x:v>6976.506</x:v>
       </x:c>
-      <x:c r="G144" t="str">
+      <x:c r="G144" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H144" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3357,7 +3790,10 @@
       <x:c r="F145" t="n">
         <x:v>4953.004</x:v>
       </x:c>
-      <x:c r="G145" t="str">
+      <x:c r="G145" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H145" t="str">
         <x:v>70.90</x:v>
       </x:c>
     </x:row>
@@ -3380,7 +3816,10 @@
       <x:c r="F146" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G146" t="str">
+      <x:c r="G146" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="H146" t="str">
         <x:v>62.33</x:v>
       </x:c>
     </x:row>
@@ -3403,7 +3842,10 @@
       <x:c r="F147" t="n">
         <x:v>11830.897</x:v>
       </x:c>
-      <x:c r="G147" t="str">
+      <x:c r="G147" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H147" t="str">
         <x:v>71.45</x:v>
       </x:c>
     </x:row>
@@ -3426,7 +3868,10 @@
       <x:c r="F148" t="n">
         <x:v>8464.870</x:v>
       </x:c>
-      <x:c r="G148" t="str">
+      <x:c r="G148" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H148" t="str">
         <x:v>81.92</x:v>
       </x:c>
     </x:row>
@@ -3449,7 +3894,10 @@
       <x:c r="F149" t="n">
         <x:v>4750.000</x:v>
       </x:c>
-      <x:c r="G149" t="str">
+      <x:c r="G149" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H149" t="str">
         <x:v>87.70</x:v>
       </x:c>
     </x:row>
@@ -3472,7 +3920,10 @@
       <x:c r="F150" t="n">
         <x:v>3307.715</x:v>
       </x:c>
-      <x:c r="G150" t="str">
+      <x:c r="G150" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H150" t="str">
         <x:v>90.87</x:v>
       </x:c>
     </x:row>
@@ -3495,7 +3946,10 @@
       <x:c r="F151" t="n">
         <x:v>5472.466</x:v>
       </x:c>
-      <x:c r="G151" t="str">
+      <x:c r="G151" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H151" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -3518,7 +3972,10 @@
       <x:c r="F152" t="n">
         <x:v>7241.491</x:v>
       </x:c>
-      <x:c r="G152" t="str">
+      <x:c r="G152" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H152" t="str">
         <x:v>81.33</x:v>
       </x:c>
     </x:row>
@@ -3541,7 +3998,10 @@
       <x:c r="F153" t="n">
         <x:v>3007.715</x:v>
       </x:c>
-      <x:c r="G153" t="str">
+      <x:c r="G153" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H153" t="str">
         <x:v>90.87</x:v>
       </x:c>
     </x:row>
@@ -3564,7 +4024,10 @@
       <x:c r="F154" t="n">
         <x:v>5120.505</x:v>
       </x:c>
-      <x:c r="G154" t="str">
+      <x:c r="G154" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H154" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -3587,7 +4050,10 @@
       <x:c r="F155" t="n">
         <x:v>7884.910</x:v>
       </x:c>
-      <x:c r="G155" t="str">
+      <x:c r="G155" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H155" t="str">
         <x:v>81.33</x:v>
       </x:c>
     </x:row>
@@ -3610,7 +4076,10 @@
       <x:c r="F156" t="n">
         <x:v>18778.629</x:v>
       </x:c>
-      <x:c r="G156" t="str">
+      <x:c r="G156" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H156" t="str">
         <x:v>77.72</x:v>
       </x:c>
     </x:row>
@@ -3633,7 +4102,10 @@
       <x:c r="F157" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G157" t="str">
+      <x:c r="G157" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="H157" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -3656,7 +4128,10 @@
       <x:c r="F158" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G158" t="str">
+      <x:c r="G158" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="H158" t="str">
         <x:v>72.65</x:v>
       </x:c>
     </x:row>
@@ -3679,7 +4154,10 @@
       <x:c r="F159" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G159" t="str">
+      <x:c r="G159" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="H159" t="str">
         <x:v>77.97</x:v>
       </x:c>
     </x:row>
@@ -3702,7 +4180,10 @@
       <x:c r="F160" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G160" t="str">
+      <x:c r="G160" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H160" t="str">
         <x:v>82.52</x:v>
       </x:c>
     </x:row>
@@ -3725,7 +4206,10 @@
       <x:c r="F161" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G161" t="str">
+      <x:c r="G161" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="H161" t="str">
         <x:v>79.08</x:v>
       </x:c>
     </x:row>
@@ -3748,7 +4232,10 @@
       <x:c r="F162" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G162" t="str">
+      <x:c r="G162" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H162" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -3771,7 +4258,10 @@
       <x:c r="F163" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G163" t="str">
+      <x:c r="G163" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H163" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -3794,7 +4284,10 @@
       <x:c r="F164" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G164" t="str">
+      <x:c r="G164" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H164" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -3817,7 +4310,10 @@
       <x:c r="F165" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G165" t="str">
+      <x:c r="G165" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="H165" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -3840,7 +4336,10 @@
       <x:c r="F166" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G166" t="str">
+      <x:c r="G166" t="n">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H166" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -3863,7 +4362,10 @@
       <x:c r="F167" t="n">
         <x:v>8465.297</x:v>
       </x:c>
-      <x:c r="G167" t="str">
+      <x:c r="G167" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H167" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -3886,7 +4388,10 @@
       <x:c r="F168" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G168" t="str">
+      <x:c r="G168" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H168" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -3909,7 +4414,10 @@
       <x:c r="F169" t="n">
         <x:v>6974.644</x:v>
       </x:c>
-      <x:c r="G169" t="str">
+      <x:c r="G169" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H169" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -3932,7 +4440,10 @@
       <x:c r="F170" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G170" t="str">
+      <x:c r="G170" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H170" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -3955,7 +4466,10 @@
       <x:c r="F171" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G171" t="str">
+      <x:c r="G171" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H171" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -3978,7 +4492,10 @@
       <x:c r="F172" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G172" t="str">
+      <x:c r="G172" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="H172" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4001,7 +4518,10 @@
       <x:c r="F173" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G173" t="str">
+      <x:c r="G173" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="H173" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -4024,7 +4544,10 @@
       <x:c r="F174" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G174" t="str">
+      <x:c r="G174" t="n">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H174" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -4047,7 +4570,10 @@
       <x:c r="F175" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G175" t="str">
+      <x:c r="G175" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H175" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -4070,7 +4596,10 @@
       <x:c r="F176" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G176" t="str">
+      <x:c r="G176" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H176" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -4093,7 +4622,10 @@
       <x:c r="F177" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G177" t="str">
+      <x:c r="G177" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H177" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -4116,7 +4648,10 @@
       <x:c r="F178" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G178" t="str">
+      <x:c r="G178" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H178" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -4139,7 +4674,10 @@
       <x:c r="F179" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G179" t="str">
+      <x:c r="G179" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H179" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -4162,7 +4700,10 @@
       <x:c r="F180" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G180" t="str">
+      <x:c r="G180" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H180" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4185,7 +4726,10 @@
       <x:c r="F181" t="n">
         <x:v>5597.386</x:v>
       </x:c>
-      <x:c r="G181" t="str">
+      <x:c r="G181" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="H181" t="str">
         <x:v>70.18</x:v>
       </x:c>
     </x:row>
@@ -4208,7 +4752,10 @@
       <x:c r="F182" t="n">
         <x:v>2947.000</x:v>
       </x:c>
-      <x:c r="G182" t="str">
+      <x:c r="G182" t="n">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H182" t="str">
         <x:v>72.07</x:v>
       </x:c>
     </x:row>
@@ -4231,7 +4778,10 @@
       <x:c r="F183" t="n">
         <x:v>8465.296</x:v>
       </x:c>
-      <x:c r="G183" t="str">
+      <x:c r="G183" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H183" t="str">
         <x:v>77.25</x:v>
       </x:c>
     </x:row>
@@ -4254,7 +4804,10 @@
       <x:c r="F184" t="n">
         <x:v>3212.544</x:v>
       </x:c>
-      <x:c r="G184" t="str">
+      <x:c r="G184" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H184" t="str">
         <x:v>79.30</x:v>
       </x:c>
     </x:row>
@@ -4277,7 +4830,10 @@
       <x:c r="F185" t="n">
         <x:v>6974.645</x:v>
       </x:c>
-      <x:c r="G185" t="str">
+      <x:c r="G185" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H185" t="str">
         <x:v>78.50</x:v>
       </x:c>
     </x:row>
@@ -4300,7 +4856,10 @@
       <x:c r="F186" t="n">
         <x:v>1328.360</x:v>
       </x:c>
-      <x:c r="G186" t="str">
+      <x:c r="G186" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H186" t="str">
         <x:v>88.65</x:v>
       </x:c>
     </x:row>
@@ -4323,7 +4882,10 @@
       <x:c r="F187" t="n">
         <x:v>7555.360</x:v>
       </x:c>
-      <x:c r="G187" t="str">
+      <x:c r="G187" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H187" t="str">
         <x:v>84.50</x:v>
       </x:c>
     </x:row>
@@ -4346,7 +4908,10 @@
       <x:c r="F188" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G188" t="str">
+      <x:c r="G188" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H188" t="str">
         <x:v>50.62</x:v>
       </x:c>
     </x:row>
@@ -4369,7 +4934,10 @@
       <x:c r="F189" t="n">
         <x:v>4800.000</x:v>
       </x:c>
-      <x:c r="G189" t="str">
+      <x:c r="G189" t="n">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="H189" t="str">
         <x:v>61.70</x:v>
       </x:c>
     </x:row>
@@ -4392,7 +4960,10 @@
       <x:c r="F190" t="n">
         <x:v>5853.750</x:v>
       </x:c>
-      <x:c r="G190" t="str">
+      <x:c r="G190" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H190" t="str">
         <x:v>71.77</x:v>
       </x:c>
     </x:row>
@@ -4415,7 +4986,10 @@
       <x:c r="F191" t="n">
         <x:v>4956.000</x:v>
       </x:c>
-      <x:c r="G191" t="str">
+      <x:c r="G191" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H191" t="str">
         <x:v>76.70</x:v>
       </x:c>
     </x:row>
@@ -4438,7 +5012,10 @@
       <x:c r="F192" t="n">
         <x:v>5424.940</x:v>
       </x:c>
-      <x:c r="G192" t="str">
+      <x:c r="G192" t="n">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="H192" t="str">
         <x:v>47.08</x:v>
       </x:c>
     </x:row>
@@ -4461,7 +5038,10 @@
       <x:c r="F193" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G193" t="str">
+      <x:c r="G193" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H193" t="str">
         <x:v>74.80</x:v>
       </x:c>
     </x:row>
@@ -4484,7 +5064,10 @@
       <x:c r="F194" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G194" t="str">
+      <x:c r="G194" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="H194" t="str">
         <x:v>74.83</x:v>
       </x:c>
     </x:row>
@@ -4507,7 +5090,10 @@
       <x:c r="F195" t="n">
         <x:v>3500.000</x:v>
       </x:c>
-      <x:c r="G195" t="str">
+      <x:c r="G195" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H195" t="str">
         <x:v>84.37</x:v>
       </x:c>
     </x:row>
@@ -4530,7 +5116,10 @@
       <x:c r="F196" t="n">
         <x:v>3500.000</x:v>
       </x:c>
-      <x:c r="G196" t="str">
+      <x:c r="G196" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H196" t="str">
         <x:v>82.13</x:v>
       </x:c>
     </x:row>
@@ -4553,7 +5142,10 @@
       <x:c r="F197" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G197" t="str">
+      <x:c r="G197" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="H197" t="str">
         <x:v>73.05</x:v>
       </x:c>
     </x:row>
@@ -4576,7 +5168,10 @@
       <x:c r="F198" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G198" t="str">
+      <x:c r="G198" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H198" t="str">
         <x:v>77.72</x:v>
       </x:c>
     </x:row>
@@ -4599,7 +5194,10 @@
       <x:c r="F199" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G199" t="str">
+      <x:c r="G199" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="H199" t="str">
         <x:v>54.95</x:v>
       </x:c>
     </x:row>
@@ -4622,7 +5220,10 @@
       <x:c r="F200" t="n">
         <x:v>4043.000</x:v>
       </x:c>
-      <x:c r="G200" t="str">
+      <x:c r="G200" t="n">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="H200" t="str">
         <x:v>52.30</x:v>
       </x:c>
     </x:row>
@@ -4645,7 +5246,10 @@
       <x:c r="F201" t="n">
         <x:v>11850.000</x:v>
       </x:c>
-      <x:c r="G201" t="str">
+      <x:c r="G201" t="n">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="H201" t="str">
         <x:v>58.90</x:v>
       </x:c>
     </x:row>
@@ -4668,7 +5272,10 @@
       <x:c r="F202" t="n">
         <x:v>11447.317</x:v>
       </x:c>
-      <x:c r="G202" t="str">
+      <x:c r="G202" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H202" t="str">
         <x:v>81.57</x:v>
       </x:c>
     </x:row>
@@ -4691,7 +5298,10 @@
       <x:c r="F203" t="n">
         <x:v>7159.229</x:v>
       </x:c>
-      <x:c r="G203" t="str">
+      <x:c r="G203" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H203" t="str">
         <x:v>93.37</x:v>
       </x:c>
     </x:row>
@@ -4714,7 +5324,10 @@
       <x:c r="F204" t="n">
         <x:v>18778.629</x:v>
       </x:c>
-      <x:c r="G204" t="str">
+      <x:c r="G204" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="H204" t="str">
         <x:v>91.18</x:v>
       </x:c>
     </x:row>
@@ -4737,7 +5350,10 @@
       <x:c r="F205" t="n">
         <x:v>3100.000</x:v>
       </x:c>
-      <x:c r="G205" t="str">
+      <x:c r="G205" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H205" t="str">
         <x:v>78.00</x:v>
       </x:c>
     </x:row>
@@ -4760,7 +5376,10 @@
       <x:c r="F206" t="n">
         <x:v>2100.000</x:v>
       </x:c>
-      <x:c r="G206" t="str">
+      <x:c r="G206" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="H206" t="str">
         <x:v>79.68</x:v>
       </x:c>
     </x:row>
@@ -4783,7 +5402,10 @@
       <x:c r="F207" t="n">
         <x:v>4135.930</x:v>
       </x:c>
-      <x:c r="G207" t="str">
+      <x:c r="G207" t="n">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="H207" t="str">
         <x:v>63.63</x:v>
       </x:c>
     </x:row>
@@ -4806,7 +5428,10 @@
       <x:c r="F208" t="n">
         <x:v>3606.000</x:v>
       </x:c>
-      <x:c r="G208" t="str">
+      <x:c r="G208" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="H208" t="str">
         <x:v>75.05</x:v>
       </x:c>
     </x:row>
@@ -4829,7 +5454,10 @@
       <x:c r="F209" t="n">
         <x:v>11228.319</x:v>
       </x:c>
-      <x:c r="G209" t="str">
+      <x:c r="G209" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H209" t="str">
         <x:v>77.78</x:v>
       </x:c>
     </x:row>
@@ -4852,7 +5480,10 @@
       <x:c r="F210" t="n">
         <x:v>8266.000</x:v>
       </x:c>
-      <x:c r="G210" t="str">
+      <x:c r="G210" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H210" t="str">
         <x:v>79.33</x:v>
       </x:c>
     </x:row>
@@ -4875,7 +5506,10 @@
       <x:c r="F211" t="n">
         <x:v>9577.269</x:v>
       </x:c>
-      <x:c r="G211" t="str">
+      <x:c r="G211" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H211" t="str">
         <x:v>78.90</x:v>
       </x:c>
     </x:row>
@@ -4898,7 +5532,10 @@
       <x:c r="F212" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G212" t="str">
+      <x:c r="G212" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H212" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -4921,7 +5558,10 @@
       <x:c r="F213" t="n">
         <x:v>3032.809</x:v>
       </x:c>
-      <x:c r="G213" t="str">
+      <x:c r="G213" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="H213" t="str">
         <x:v>48.28</x:v>
       </x:c>
     </x:row>
@@ -4944,7 +5584,10 @@
       <x:c r="F214" t="n">
         <x:v>6013.366</x:v>
       </x:c>
-      <x:c r="G214" t="str">
+      <x:c r="G214" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="H214" t="str">
         <x:v>57.85</x:v>
       </x:c>
     </x:row>
@@ -4967,7 +5610,10 @@
       <x:c r="F215" t="n">
         <x:v>1999.000</x:v>
       </x:c>
-      <x:c r="G215" t="str">
+      <x:c r="G215" t="n">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="H215" t="str">
         <x:v>50.33</x:v>
       </x:c>
     </x:row>
@@ -4990,7 +5636,10 @@
       <x:c r="F216" t="n">
         <x:v>7959.844</x:v>
       </x:c>
-      <x:c r="G216" t="str">
+      <x:c r="G216" t="n">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="H216" t="str">
         <x:v>49.57</x:v>
       </x:c>
     </x:row>
@@ -5013,7 +5662,10 @@
       <x:c r="F217" t="n">
         <x:v>1876.448</x:v>
       </x:c>
-      <x:c r="G217" t="str">
+      <x:c r="G217" t="n">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="H217" t="str">
         <x:v>55.58</x:v>
       </x:c>
     </x:row>
@@ -5036,7 +5688,10 @@
       <x:c r="F218" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G218" t="str">
+      <x:c r="G218" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H218" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5059,7 +5714,10 @@
       <x:c r="F219" t="n">
         <x:v>1932.039</x:v>
       </x:c>
-      <x:c r="G219" t="str">
+      <x:c r="G219" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H219" t="str">
         <x:v>65.22</x:v>
       </x:c>
     </x:row>
@@ -5082,7 +5740,10 @@
       <x:c r="F220" t="n">
         <x:v>4067.961</x:v>
       </x:c>
-      <x:c r="G220" t="str">
+      <x:c r="G220" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H220" t="str">
         <x:v>71.78</x:v>
       </x:c>
     </x:row>
@@ -5105,7 +5766,10 @@
       <x:c r="F221" t="n">
         <x:v>8649.557</x:v>
       </x:c>
-      <x:c r="G221" t="str">
+      <x:c r="G221" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H221" t="str">
         <x:v>67.80</x:v>
       </x:c>
     </x:row>
@@ -5128,7 +5792,10 @@
       <x:c r="F222" t="n">
         <x:v>8649.557</x:v>
       </x:c>
-      <x:c r="G222" t="str">
+      <x:c r="G222" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="H222" t="str">
         <x:v>70.63</x:v>
       </x:c>
     </x:row>
@@ -5151,7 +5818,10 @@
       <x:c r="F223" t="n">
         <x:v>23663.000</x:v>
       </x:c>
-      <x:c r="G223" t="str">
+      <x:c r="G223" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H223" t="str">
         <x:v>68.13</x:v>
       </x:c>
     </x:row>
@@ -5174,7 +5844,10 @@
       <x:c r="F224" t="n">
         <x:v>5779.193</x:v>
       </x:c>
-      <x:c r="G224" t="str">
+      <x:c r="G224" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="H224" t="str">
         <x:v>77.42</x:v>
       </x:c>
     </x:row>
@@ -5197,7 +5870,10 @@
       <x:c r="F225" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G225" t="str">
+      <x:c r="G225" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="H225" t="str">
         <x:v>67.45</x:v>
       </x:c>
     </x:row>
@@ -5220,7 +5896,10 @@
       <x:c r="F226" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G226" t="str">
+      <x:c r="G226" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H226" t="str">
         <x:v>70.32</x:v>
       </x:c>
     </x:row>
@@ -5243,7 +5922,10 @@
       <x:c r="F227" t="n">
         <x:v>1006.000</x:v>
       </x:c>
-      <x:c r="G227" t="str">
+      <x:c r="G227" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="H227" t="str">
         <x:v>54.05</x:v>
       </x:c>
     </x:row>
@@ -5266,7 +5948,10 @@
       <x:c r="F228" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G228" t="str">
+      <x:c r="G228" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="H228" t="str">
         <x:v>62.68</x:v>
       </x:c>
     </x:row>
@@ -5289,7 +5974,10 @@
       <x:c r="F229" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G229" t="str">
+      <x:c r="G229" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H229" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5312,7 +6000,10 @@
       <x:c r="F230" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G230" t="str">
+      <x:c r="G230" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H230" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5335,7 +6026,10 @@
       <x:c r="F231" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G231" t="str">
+      <x:c r="G231" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H231" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5358,7 +6052,10 @@
       <x:c r="F232" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G232" t="str">
+      <x:c r="G232" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H232" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5381,7 +6078,10 @@
       <x:c r="F233" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G233" t="str">
+      <x:c r="G233" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H233" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5404,7 +6104,10 @@
       <x:c r="F234" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G234" t="str">
+      <x:c r="G234" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H234" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5427,7 +6130,10 @@
       <x:c r="F235" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G235" t="str">
+      <x:c r="G235" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H235" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5450,7 +6156,10 @@
       <x:c r="F236" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G236" t="str">
+      <x:c r="G236" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H236" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5473,7 +6182,10 @@
       <x:c r="F237" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G237" t="str">
+      <x:c r="G237" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H237" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5496,7 +6208,10 @@
       <x:c r="F238" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G238" t="str">
+      <x:c r="G238" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H238" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5519,7 +6234,10 @@
       <x:c r="F239" t="n">
         <x:v>3400.000</x:v>
       </x:c>
-      <x:c r="G239" t="str">
+      <x:c r="G239" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H239" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5542,7 +6260,10 @@
       <x:c r="F240" t="n">
         <x:v>6913.550</x:v>
       </x:c>
-      <x:c r="G240" t="str">
+      <x:c r="G240" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H240" t="str">
         <x:v>72.50</x:v>
       </x:c>
     </x:row>
@@ -5565,7 +6286,10 @@
       <x:c r="F241" t="n">
         <x:v>3103.004</x:v>
       </x:c>
-      <x:c r="G241" t="str">
+      <x:c r="G241" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H241" t="str">
         <x:v>62.83</x:v>
       </x:c>
     </x:row>
@@ -5588,7 +6312,10 @@
       <x:c r="F242" t="n">
         <x:v>5703.603</x:v>
       </x:c>
-      <x:c r="G242" t="str">
+      <x:c r="G242" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H242" t="str">
         <x:v>68.75</x:v>
       </x:c>
     </x:row>
@@ -5611,7 +6338,10 @@
       <x:c r="F243" t="n">
         <x:v>3278.000</x:v>
       </x:c>
-      <x:c r="G243" t="str">
+      <x:c r="G243" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H243" t="str">
         <x:v>61.28</x:v>
       </x:c>
     </x:row>
@@ -5634,7 +6364,10 @@
       <x:c r="F244" t="n">
         <x:v>1037.693</x:v>
       </x:c>
-      <x:c r="G244" t="str">
+      <x:c r="G244" t="n">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="H244" t="str">
         <x:v>61.67</x:v>
       </x:c>
     </x:row>
@@ -5657,7 +6390,10 @@
       <x:c r="F245" t="n">
         <x:v>7243.000</x:v>
       </x:c>
-      <x:c r="G245" t="str">
+      <x:c r="G245" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H245" t="str">
         <x:v>77.87</x:v>
       </x:c>
     </x:row>
@@ -5680,7 +6416,10 @@
       <x:c r="F246" t="n">
         <x:v>13334.725</x:v>
       </x:c>
-      <x:c r="G246" t="str">
+      <x:c r="G246" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="H246" t="str">
         <x:v>77.87</x:v>
       </x:c>
     </x:row>
@@ -5703,7 +6442,10 @@
       <x:c r="F247" t="n">
         <x:v>14867.031</x:v>
       </x:c>
-      <x:c r="G247" t="str">
+      <x:c r="G247" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H247" t="str">
         <x:v>90.17</x:v>
       </x:c>
     </x:row>
@@ -5726,7 +6468,10 @@
       <x:c r="F248" t="n">
         <x:v>3479.273</x:v>
       </x:c>
-      <x:c r="G248" t="str">
+      <x:c r="G248" t="n">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="H248" t="str">
         <x:v>63.43</x:v>
       </x:c>
     </x:row>
@@ -5749,7 +6494,10 @@
       <x:c r="F249" t="n">
         <x:v>2807.996</x:v>
       </x:c>
-      <x:c r="G249" t="str">
+      <x:c r="G249" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H249" t="str">
         <x:v>92.03</x:v>
       </x:c>
     </x:row>
@@ -5772,7 +6520,10 @@
       <x:c r="F250" t="n">
         <x:v>1706.000</x:v>
       </x:c>
-      <x:c r="G250" t="str">
+      <x:c r="G250" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H250" t="str">
         <x:v>48.78</x:v>
       </x:c>
     </x:row>
@@ -5795,7 +6546,10 @@
       <x:c r="F251" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G251" t="str">
+      <x:c r="G251" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="H251" t="str">
         <x:v>40.02</x:v>
       </x:c>
     </x:row>
@@ -5818,7 +6572,10 @@
       <x:c r="F252" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G252" t="str">
+      <x:c r="G252" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="H252" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5841,7 +6598,10 @@
       <x:c r="F253" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G253" t="str">
+      <x:c r="G253" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="H253" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5864,7 +6624,10 @@
       <x:c r="F254" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G254" t="str">
+      <x:c r="G254" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="H254" t="str">
         <x:v>28.45</x:v>
       </x:c>
     </x:row>
@@ -5887,7 +6650,10 @@
       <x:c r="F255" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G255" t="str">
+      <x:c r="G255" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="H255" t="str">
         <x:v>33.33</x:v>
       </x:c>
     </x:row>
@@ -5910,7 +6676,10 @@
       <x:c r="F256" t="n">
         <x:v>2006.000</x:v>
       </x:c>
-      <x:c r="G256" t="str">
+      <x:c r="G256" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="H256" t="str">
         <x:v>33.33</x:v>
       </x:c>
     </x:row>
@@ -5933,7 +6702,10 @@
       <x:c r="F257" t="n">
         <x:v>906.000</x:v>
       </x:c>
-      <x:c r="G257" t="str">
+      <x:c r="G257" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="H257" t="str">
         <x:v>28.60</x:v>
       </x:c>
     </x:row>
@@ -5956,7 +6728,10 @@
       <x:c r="F258" t="n">
         <x:v>1206.000</x:v>
       </x:c>
-      <x:c r="G258" t="str">
+      <x:c r="G258" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H258" t="str">
         <x:v>37.68</x:v>
       </x:c>
     </x:row>
@@ -5979,7 +6754,10 @@
       <x:c r="F259" t="n">
         <x:v>1556.000</x:v>
       </x:c>
-      <x:c r="G259" t="str">
+      <x:c r="G259" t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="H259" t="str">
         <x:v>54.53</x:v>
       </x:c>
     </x:row>
@@ -6002,7 +6780,10 @@
       <x:c r="F260" t="n">
         <x:v>1917.000</x:v>
       </x:c>
-      <x:c r="G260" t="str">
+      <x:c r="G260" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="H260" t="str">
         <x:v>50.92</x:v>
       </x:c>
     </x:row>
@@ -6025,7 +6806,10 @@
       <x:c r="F261" t="n">
         <x:v>6726.984</x:v>
       </x:c>
-      <x:c r="G261" t="str">
+      <x:c r="G261" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H261" t="str">
         <x:v>61.32</x:v>
       </x:c>
     </x:row>
@@ -6048,7 +6832,10 @@
       <x:c r="F262" t="n">
         <x:v>3147.000</x:v>
       </x:c>
-      <x:c r="G262" t="str">
+      <x:c r="G262" t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H262" t="str">
         <x:v>53.27</x:v>
       </x:c>
     </x:row>
@@ -6071,7 +6858,10 @@
       <x:c r="F263" t="n">
         <x:v>3518.192</x:v>
       </x:c>
-      <x:c r="G263" t="str">
+      <x:c r="G263" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="H263" t="str">
         <x:v>55.25</x:v>
       </x:c>
     </x:row>
@@ -6094,7 +6884,10 @@
       <x:c r="F264" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G264" t="str">
+      <x:c r="G264" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="H264" t="str">
         <x:v>53.37</x:v>
       </x:c>
     </x:row>
@@ -6117,7 +6910,10 @@
       <x:c r="F265" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G265" t="str">
+      <x:c r="G265" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H265" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6140,7 +6936,10 @@
       <x:c r="F266" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G266" t="str">
+      <x:c r="G266" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H266" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6163,7 +6962,10 @@
       <x:c r="F267" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G267" t="str">
+      <x:c r="G267" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H267" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6186,7 +6988,10 @@
       <x:c r="F268" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G268" t="str">
+      <x:c r="G268" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H268" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6209,7 +7014,10 @@
       <x:c r="F269" t="n">
         <x:v>3800.000</x:v>
       </x:c>
-      <x:c r="G269" t="str">
+      <x:c r="G269" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H269" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6232,7 +7040,10 @@
       <x:c r="F270" t="n">
         <x:v>2350.000</x:v>
       </x:c>
-      <x:c r="G270" t="str">
+      <x:c r="G270" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H270" t="str">
         <x:v>94.37</x:v>
       </x:c>
     </x:row>
@@ -6255,7 +7066,10 @@
       <x:c r="F271" t="n">
         <x:v>2350.000</x:v>
       </x:c>
-      <x:c r="G271" t="str">
+      <x:c r="G271" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H271" t="str">
         <x:v>94.37</x:v>
       </x:c>
     </x:row>
@@ -6278,7 +7092,10 @@
       <x:c r="F272" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G272" t="str">
+      <x:c r="G272" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H272" t="str">
         <x:v>96.03</x:v>
       </x:c>
     </x:row>
@@ -6301,7 +7118,10 @@
       <x:c r="F273" t="n">
         <x:v>3956.000</x:v>
       </x:c>
-      <x:c r="G273" t="str">
+      <x:c r="G273" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="H273" t="str">
         <x:v>65.27</x:v>
       </x:c>
     </x:row>
@@ -6324,7 +7144,10 @@
       <x:c r="F274" t="n">
         <x:v>1600.000</x:v>
       </x:c>
-      <x:c r="G274" t="str">
+      <x:c r="G274" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="H274" t="str">
         <x:v>88.10</x:v>
       </x:c>
     </x:row>
@@ -6347,7 +7170,10 @@
       <x:c r="F275" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G275" t="str">
+      <x:c r="G275" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H275" t="str">
         <x:v>81.20</x:v>
       </x:c>
     </x:row>
@@ -6370,7 +7196,10 @@
       <x:c r="F276" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G276" t="str">
+      <x:c r="G276" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H276" t="str">
         <x:v>66.37</x:v>
       </x:c>
     </x:row>
@@ -6393,7 +7222,10 @@
       <x:c r="F277" t="n">
         <x:v>2413.000</x:v>
       </x:c>
-      <x:c r="G277" t="str">
+      <x:c r="G277" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H277" t="str">
         <x:v>58.95</x:v>
       </x:c>
     </x:row>
@@ -6416,7 +7248,10 @@
       <x:c r="F278" t="n">
         <x:v>6102.344</x:v>
       </x:c>
-      <x:c r="G278" t="str">
+      <x:c r="G278" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H278" t="str">
         <x:v>60.93</x:v>
       </x:c>
     </x:row>
@@ -6439,7 +7274,10 @@
       <x:c r="F279" t="n">
         <x:v>3150.000</x:v>
       </x:c>
-      <x:c r="G279" t="str">
+      <x:c r="G279" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H279" t="str">
         <x:v>97.85</x:v>
       </x:c>
     </x:row>
@@ -6462,7 +7300,10 @@
       <x:c r="F280" t="n">
         <x:v>2870.619</x:v>
       </x:c>
-      <x:c r="G280" t="str">
+      <x:c r="G280" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H280" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -6485,7 +7326,10 @@
       <x:c r="F281" t="n">
         <x:v>3603.210</x:v>
       </x:c>
-      <x:c r="G281" t="str">
+      <x:c r="G281" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="H281" t="str">
         <x:v>68.88</x:v>
       </x:c>
     </x:row>
@@ -6508,7 +7352,10 @@
       <x:c r="F282" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G282" t="str">
+      <x:c r="G282" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H282" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6531,7 +7378,10 @@
       <x:c r="F283" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G283" t="str">
+      <x:c r="G283" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H283" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6554,7 +7404,10 @@
       <x:c r="F284" t="n">
         <x:v>4953.210</x:v>
       </x:c>
-      <x:c r="G284" t="str">
+      <x:c r="G284" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="H284" t="str">
         <x:v>65.77</x:v>
       </x:c>
     </x:row>
@@ -6577,7 +7430,10 @@
       <x:c r="F285" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G285" t="str">
+      <x:c r="G285" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H285" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6600,7 +7456,10 @@
       <x:c r="F286" t="n">
         <x:v>900.000</x:v>
       </x:c>
-      <x:c r="G286" t="str">
+      <x:c r="G286" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H286" t="str">
         <x:v>84.17</x:v>
       </x:c>
     </x:row>
@@ -6623,7 +7482,10 @@
       <x:c r="F287" t="n">
         <x:v>3753.210</x:v>
       </x:c>
-      <x:c r="G287" t="str">
+      <x:c r="G287" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="H287" t="str">
         <x:v>41.15</x:v>
       </x:c>
     </x:row>
@@ -6646,7 +7508,10 @@
       <x:c r="F288" t="n">
         <x:v>1700.000</x:v>
       </x:c>
-      <x:c r="G288" t="str">
+      <x:c r="G288" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H288" t="str">
         <x:v>64.83</x:v>
       </x:c>
     </x:row>
@@ -6669,7 +7534,10 @@
       <x:c r="F289" t="n">
         <x:v>1650.000</x:v>
       </x:c>
-      <x:c r="G289" t="str">
+      <x:c r="G289" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H289" t="str">
         <x:v>91.90</x:v>
       </x:c>
     </x:row>
@@ -6692,7 +7560,10 @@
       <x:c r="F290" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G290" t="str">
+      <x:c r="G290" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="H290" t="str">
         <x:v>58.23</x:v>
       </x:c>
     </x:row>
@@ -6715,7 +7586,10 @@
       <x:c r="F291" t="n">
         <x:v>1750.000</x:v>
       </x:c>
-      <x:c r="G291" t="str">
+      <x:c r="G291" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="H291" t="str">
         <x:v>84.00</x:v>
       </x:c>
     </x:row>
@@ -6738,7 +7612,10 @@
       <x:c r="F292" t="n">
         <x:v>2153.210</x:v>
       </x:c>
-      <x:c r="G292" t="str">
+      <x:c r="G292" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="H292" t="str">
         <x:v>77.33</x:v>
       </x:c>
     </x:row>
@@ -6761,7 +7638,10 @@
       <x:c r="F293" t="n">
         <x:v>6600.000</x:v>
       </x:c>
-      <x:c r="G293" t="str">
+      <x:c r="G293" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H293" t="str">
         <x:v>73.52</x:v>
       </x:c>
     </x:row>
@@ -6784,7 +7664,10 @@
       <x:c r="F294" t="n">
         <x:v>1530.000</x:v>
       </x:c>
-      <x:c r="G294" t="str">
+      <x:c r="G294" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H294" t="str">
         <x:v>96.77</x:v>
       </x:c>
     </x:row>
@@ -6807,7 +7690,10 @@
       <x:c r="F295" t="n">
         <x:v>930.000</x:v>
       </x:c>
-      <x:c r="G295" t="str">
+      <x:c r="G295" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H295" t="str">
         <x:v>88.07</x:v>
       </x:c>
     </x:row>
@@ -6830,7 +7716,10 @@
       <x:c r="F296" t="n">
         <x:v>6000.000</x:v>
       </x:c>
-      <x:c r="G296" t="str">
+      <x:c r="G296" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H296" t="str">
         <x:v>84.13</x:v>
       </x:c>
     </x:row>
@@ -6853,7 +7742,10 @@
       <x:c r="F297" t="n">
         <x:v>3560.000</x:v>
       </x:c>
-      <x:c r="G297" t="str">
+      <x:c r="G297" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H297" t="str">
         <x:v>80.90</x:v>
       </x:c>
     </x:row>
@@ -6876,7 +7768,10 @@
       <x:c r="F298" t="n">
         <x:v>2403.772</x:v>
       </x:c>
-      <x:c r="G298" t="str">
+      <x:c r="G298" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H298" t="str">
         <x:v>77.00</x:v>
       </x:c>
     </x:row>
@@ -6899,7 +7794,10 @@
       <x:c r="F299" t="n">
         <x:v>4394.246</x:v>
       </x:c>
-      <x:c r="G299" t="str">
+      <x:c r="G299" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H299" t="str">
         <x:v>77.00</x:v>
       </x:c>
     </x:row>
@@ -6922,7 +7820,10 @@
       <x:c r="F300" t="n">
         <x:v>3855.754</x:v>
       </x:c>
-      <x:c r="G300" t="str">
+      <x:c r="G300" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H300" t="str">
         <x:v>91.60</x:v>
       </x:c>
     </x:row>
@@ -6945,7 +7846,10 @@
       <x:c r="F301" t="n">
         <x:v>2800.000</x:v>
       </x:c>
-      <x:c r="G301" t="str">
+      <x:c r="G301" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H301" t="str">
         <x:v>73.27</x:v>
       </x:c>
     </x:row>
@@ -6968,7 +7872,10 @@
       <x:c r="F302" t="n">
         <x:v>3744.215</x:v>
       </x:c>
-      <x:c r="G302" t="str">
+      <x:c r="G302" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H302" t="str">
         <x:v>77.17</x:v>
       </x:c>
     </x:row>
@@ -6991,7 +7898,10 @@
       <x:c r="F303" t="n">
         <x:v>1687.000</x:v>
       </x:c>
-      <x:c r="G303" t="str">
+      <x:c r="G303" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H303" t="str">
         <x:v>84.73</x:v>
       </x:c>
     </x:row>
@@ -7014,7 +7924,10 @@
       <x:c r="F304" t="n">
         <x:v>2200.000</x:v>
       </x:c>
-      <x:c r="G304" t="str">
+      <x:c r="G304" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H304" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -7037,7 +7950,10 @@
       <x:c r="F305" t="n">
         <x:v>8151.985</x:v>
       </x:c>
-      <x:c r="G305" t="str">
+      <x:c r="G305" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H305" t="str">
         <x:v>57.18</x:v>
       </x:c>
     </x:row>
@@ -7060,7 +7976,10 @@
       <x:c r="F306" t="n">
         <x:v>3475.911</x:v>
       </x:c>
-      <x:c r="G306" t="str">
+      <x:c r="G306" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H306" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7083,7 +8002,10 @@
       <x:c r="F307" t="n">
         <x:v>14620.000</x:v>
       </x:c>
-      <x:c r="G307" t="str">
+      <x:c r="G307" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H307" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -7106,7 +8028,10 @@
       <x:c r="F308" t="n">
         <x:v>2150.000</x:v>
       </x:c>
-      <x:c r="G308" t="str">
+      <x:c r="G308" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H308" t="str">
         <x:v>82.83</x:v>
       </x:c>
     </x:row>
@@ -7129,7 +8054,10 @@
       <x:c r="F309" t="n">
         <x:v>5101.000</x:v>
       </x:c>
-      <x:c r="G309" t="str">
+      <x:c r="G309" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H309" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -7152,7 +8080,10 @@
       <x:c r="F310" t="n">
         <x:v>6665.979</x:v>
       </x:c>
-      <x:c r="G310" t="str">
+      <x:c r="G310" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H310" t="str">
         <x:v>62.92</x:v>
       </x:c>
     </x:row>
@@ -7175,7 +8106,10 @@
       <x:c r="F311" t="n">
         <x:v>5305.587</x:v>
       </x:c>
-      <x:c r="G311" t="str">
+      <x:c r="G311" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H311" t="str">
         <x:v>100.00</x:v>
       </x:c>
     </x:row>
@@ -7198,7 +8132,10 @@
       <x:c r="F312" t="n">
         <x:v>5333.466</x:v>
       </x:c>
-      <x:c r="G312" t="str">
+      <x:c r="G312" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H312" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
@@ -7221,7 +8158,10 @@
       <x:c r="F313" t="n">
         <x:v>2787.000</x:v>
       </x:c>
-      <x:c r="G313" t="str">
+      <x:c r="G313" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H313" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
@@ -7244,7 +8184,10 @@
       <x:c r="F314" t="n">
         <x:v>3000.000</x:v>
       </x:c>
-      <x:c r="G314" t="str">
+      <x:c r="G314" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H314" t="str">
         <x:v>69.47</x:v>
       </x:c>
     </x:row>
@@ -7267,7 +8210,10 @@
       <x:c r="F315" t="n">
         <x:v>4384.000</x:v>
       </x:c>
-      <x:c r="G315" t="str">
+      <x:c r="G315" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H315" t="str">
         <x:v>84.73</x:v>
       </x:c>
     </x:row>
@@ -7290,7 +8236,10 @@
       <x:c r="F316" t="n">
         <x:v>4500.000</x:v>
       </x:c>
-      <x:c r="G316" t="str">
+      <x:c r="G316" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H316" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7313,7 +8262,10 @@
       <x:c r="F317" t="n">
         <x:v>8462.000</x:v>
       </x:c>
-      <x:c r="G317" t="str">
+      <x:c r="G317" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H317" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7336,7 +8288,10 @@
       <x:c r="F318" t="n">
         <x:v>8196.993</x:v>
       </x:c>
-      <x:c r="G318" t="str">
+      <x:c r="G318" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H318" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7359,7 +8314,10 @@
       <x:c r="F319" t="n">
         <x:v>6511.970</x:v>
       </x:c>
-      <x:c r="G319" t="str">
+      <x:c r="G319" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="H319" t="str">
         <x:v>53.25</x:v>
       </x:c>
     </x:row>
@@ -7382,13 +8340,16 @@
       <x:c r="F320" t="n">
         <x:v>6997.239</x:v>
       </x:c>
-      <x:c r="G320" t="str">
+      <x:c r="G320" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="H320" t="str">
         <x:v>61.83</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:tableParts>
-    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R44510aa9eabf489f"/>
+    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rf34cc0f2e7104504"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>